<commit_message>
Add more gftp tests and update summary doc
</commit_message>
<xml_diff>
--- a/summary_data/gftp_summary.xlsx
+++ b/summary_data/gftp_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isfiligoi/github/tnrp-net-tests/summary_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DABE8F-B316-2946-B679-13B2F2AFB2C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98022C1-A8F7-B14F-AD71-436507EA3EC0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="-26640" windowWidth="47120" windowHeight="24500" xr2:uid="{F871B44F-434F-FB4B-AC1F-99327B90C475}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="23">
   <si>
     <t>Server</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>GridFTP tests - single threaded, single process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: </t>
+  </si>
+  <si>
+    <t>When testing gridftp servers that have multiple interfaces, picking the one that is faster fo the specific test</t>
   </si>
 </sst>
 </file>
@@ -177,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -193,6 +199,7 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AE2A42-D91B-564A-AB68-339151ECBD6D}">
-  <dimension ref="A1:AF37"/>
+  <dimension ref="A1:AF44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y11" sqref="Y11"/>
+      <selection activeCell="AA43" sqref="AA43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1194,10 +1201,16 @@
       <c r="B19" t="s">
         <v>2</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="C19" s="5">
+        <v>52.8</v>
+      </c>
+      <c r="D19" s="5">
+        <v>3.29</v>
+      </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
+      <c r="F19" s="5">
+        <v>52.7</v>
+      </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -1211,10 +1224,19 @@
         <f>B19</f>
         <v>AWS EU C1</v>
       </c>
-      <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
+      <c r="T19" s="6">
+        <f>100/C19</f>
+        <v>1.893939393939394</v>
+      </c>
+      <c r="U19" s="13">
+        <f t="shared" ref="U19:V21" si="0">100/D19</f>
+        <v>30.3951367781155</v>
+      </c>
       <c r="V19" s="5"/>
-      <c r="W19" s="5"/>
+      <c r="W19" s="6">
+        <f t="shared" ref="W19:W24" si="1">100/F19</f>
+        <v>1.8975332068311195</v>
+      </c>
       <c r="X19" s="5"/>
       <c r="Y19" s="5"/>
       <c r="Z19" s="5"/>
@@ -1247,7 +1269,9 @@
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
+      <c r="M20" s="5">
+        <v>23.5</v>
+      </c>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="S20" t="str">
@@ -1259,12 +1283,12 @@
         <v>9.3457943925233646</v>
       </c>
       <c r="U20" s="6">
-        <f t="shared" ref="U20:U21" si="0">100/D20</f>
+        <f t="shared" si="0"/>
         <v>9.5238095238095237</v>
       </c>
       <c r="V20" s="6"/>
       <c r="W20" s="6">
-        <f t="shared" ref="W20:W24" si="1">100/F20</f>
+        <f t="shared" si="1"/>
         <v>3.1446540880503142</v>
       </c>
       <c r="X20" s="6">
@@ -1276,7 +1300,10 @@
       <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
       <c r="AC20" s="6"/>
-      <c r="AD20" s="6"/>
+      <c r="AD20" s="6">
+        <f t="shared" ref="AC20:AD24" si="3">100/M20</f>
+        <v>4.2553191489361701</v>
+      </c>
       <c r="AE20" s="6"/>
       <c r="AF20" s="6"/>
     </row>
@@ -1316,15 +1343,15 @@
         <v>NewYork</v>
       </c>
       <c r="T21" s="6">
-        <f t="shared" ref="T21" si="3">100/C21</f>
+        <f t="shared" ref="T21" si="4">100/C21</f>
         <v>1.0834236186348862</v>
       </c>
       <c r="U21" s="6">
         <f t="shared" si="0"/>
         <v>1.0893246187363834</v>
       </c>
-      <c r="V21" s="6">
-        <f t="shared" ref="V20:V21" si="4">100/E21</f>
+      <c r="V21" s="11">
+        <f t="shared" si="0"/>
         <v>3.4482758620689653</v>
       </c>
       <c r="W21" s="13">
@@ -1343,7 +1370,7 @@
       </c>
       <c r="AB21" s="6"/>
       <c r="AC21" s="6">
-        <f t="shared" ref="AC21:AC24" si="6">100/L21</f>
+        <f t="shared" si="3"/>
         <v>2.7700831024930745</v>
       </c>
       <c r="AD21" s="6"/>
@@ -1396,7 +1423,9 @@
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="E23" s="5">
+        <v>21.6</v>
+      </c>
       <c r="F23" s="5">
         <v>25.5</v>
       </c>
@@ -1416,7 +1445,9 @@
       <c r="L23" s="5">
         <v>12.8</v>
       </c>
-      <c r="M23" s="5"/>
+      <c r="M23" s="5">
+        <v>50.8</v>
+      </c>
       <c r="N23" s="5"/>
       <c r="O23" s="5"/>
       <c r="S23" t="str">
@@ -1425,7 +1456,10 @@
       </c>
       <c r="T23" s="6"/>
       <c r="U23" s="6"/>
-      <c r="V23" s="6"/>
+      <c r="V23" s="11">
+        <f t="shared" ref="V23" si="6">100/E23</f>
+        <v>4.6296296296296298</v>
+      </c>
       <c r="W23" s="6">
         <f t="shared" si="1"/>
         <v>3.9215686274509802</v>
@@ -1448,10 +1482,13 @@
         <v>6.1349693251533743</v>
       </c>
       <c r="AC23" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>7.8125</v>
       </c>
-      <c r="AD23" s="6"/>
+      <c r="AD23" s="6">
+        <f t="shared" si="3"/>
+        <v>1.9685039370078741</v>
+      </c>
       <c r="AE23" s="6"/>
       <c r="AF23" s="6"/>
     </row>
@@ -1493,7 +1530,7 @@
       <c r="AA24" s="6"/>
       <c r="AB24" s="6"/>
       <c r="AC24" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>5.9880239520958085</v>
       </c>
       <c r="AD24" s="6"/>
@@ -1645,10 +1682,16 @@
       <c r="B32" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
+      <c r="C32" s="7">
+        <v>167</v>
+      </c>
+      <c r="D32" s="7">
+        <v>8.6</v>
+      </c>
       <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+      <c r="F32" s="7">
+        <v>566</v>
+      </c>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
@@ -1662,10 +1705,19 @@
         <f>B32</f>
         <v>AWS EU C1</v>
       </c>
-      <c r="T32" s="7"/>
-      <c r="U32" s="7"/>
+      <c r="T32" s="12">
+        <f>100/C32</f>
+        <v>0.59880239520958078</v>
+      </c>
+      <c r="U32" s="15">
+        <f t="shared" ref="U32:U34" si="9">100/D32</f>
+        <v>11.627906976744187</v>
+      </c>
       <c r="V32" s="7"/>
-      <c r="W32" s="7"/>
+      <c r="W32" s="12">
+        <f t="shared" ref="W32:W37" si="10">100/F32</f>
+        <v>0.17667844522968199</v>
+      </c>
       <c r="X32" s="7"/>
       <c r="Y32" s="7"/>
       <c r="Z32" s="7"/>
@@ -1676,7 +1728,7 @@
       <c r="AE32" s="7"/>
       <c r="AF32" s="7"/>
     </row>
-    <row r="33" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>3</v>
       </c>
@@ -1698,7 +1750,9 @@
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
+      <c r="M33" s="7">
+        <v>163</v>
+      </c>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
       <c r="S33" t="str">
@@ -1710,12 +1764,12 @@
         <v>0.65359477124183007</v>
       </c>
       <c r="U33" s="11">
-        <f t="shared" ref="U33:U34" si="9">100/D33</f>
+        <f t="shared" si="9"/>
         <v>2.1413276231263381</v>
       </c>
       <c r="V33" s="11"/>
       <c r="W33" s="12">
-        <f t="shared" ref="W33:W37" si="10">100/F33</f>
+        <f t="shared" si="10"/>
         <v>0.16583747927031509</v>
       </c>
       <c r="X33" s="11">
@@ -1727,11 +1781,14 @@
       <c r="AA33" s="11"/>
       <c r="AB33" s="11"/>
       <c r="AC33" s="11"/>
-      <c r="AD33" s="11"/>
+      <c r="AD33" s="11">
+        <f t="shared" ref="AD33" si="12">100/M33</f>
+        <v>0.61349693251533743</v>
+      </c>
       <c r="AE33" s="11"/>
       <c r="AF33" s="11"/>
     </row>
-    <row r="34" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>13</v>
       </c>
@@ -1767,7 +1824,7 @@
         <v>NewYork</v>
       </c>
       <c r="T34" s="12">
-        <f t="shared" ref="T34" si="12">100/C34</f>
+        <f t="shared" ref="T34" si="13">100/C34</f>
         <v>0.14836795252225518</v>
       </c>
       <c r="U34" s="12">
@@ -1775,33 +1832,33 @@
         <v>0.17006802721088435</v>
       </c>
       <c r="V34" s="11">
-        <f t="shared" ref="V34:V35" si="13">100/E34</f>
+        <f t="shared" ref="V34:V36" si="14">100/E34</f>
         <v>1.2048192771084338</v>
       </c>
       <c r="W34" s="11">
         <f t="shared" si="10"/>
         <v>2.2271714922048997</v>
       </c>
-      <c r="X34" s="11">
+      <c r="X34" s="15">
         <f t="shared" si="11"/>
         <v>10.989010989010989</v>
       </c>
       <c r="Y34" s="11"/>
       <c r="Z34" s="11"/>
       <c r="AA34" s="12">
-        <f t="shared" ref="AA34:AA36" si="14">100/J34</f>
+        <f t="shared" ref="AA34:AA36" si="15">100/J34</f>
         <v>0.4329004329004329</v>
       </c>
       <c r="AB34" s="11"/>
       <c r="AC34" s="12">
-        <f t="shared" ref="AC34:AC37" si="15">100/L34</f>
+        <f t="shared" ref="AC34:AC37" si="16">100/L34</f>
         <v>0.12376237623762376</v>
       </c>
       <c r="AD34" s="11"/>
       <c r="AE34" s="11"/>
       <c r="AF34" s="11"/>
     </row>
-    <row r="35" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>8</v>
       </c>
@@ -1841,13 +1898,15 @@
       <c r="AE35" s="11"/>
       <c r="AF35" s="11"/>
     </row>
-    <row r="36" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>6</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
+      <c r="E36" s="7">
+        <v>21.6</v>
+      </c>
       <c r="F36" s="7">
         <v>463</v>
       </c>
@@ -1867,7 +1926,9 @@
       <c r="L36" s="7">
         <v>232</v>
       </c>
-      <c r="M36" s="7"/>
+      <c r="M36" s="7">
+        <v>87.4</v>
+      </c>
       <c r="N36" s="7"/>
       <c r="O36" s="7"/>
       <c r="S36" t="str">
@@ -1876,37 +1937,43 @@
       </c>
       <c r="T36" s="11"/>
       <c r="U36" s="11"/>
-      <c r="V36" s="11"/>
+      <c r="V36" s="11">
+        <f t="shared" si="14"/>
+        <v>4.6296296296296298</v>
+      </c>
       <c r="W36" s="12">
         <f t="shared" si="10"/>
         <v>0.21598272138228941</v>
       </c>
       <c r="X36" s="11">
-        <f t="shared" ref="X36:X37" si="16">100/G36</f>
+        <f t="shared" ref="X36:X37" si="17">100/G36</f>
         <v>7.9365079365079367</v>
       </c>
       <c r="Y36" s="11"/>
-      <c r="Z36" s="11">
-        <f t="shared" ref="Z36" si="17">100/I36</f>
+      <c r="Z36" s="15">
+        <f t="shared" ref="Z36" si="18">100/I36</f>
         <v>17.361111111111111</v>
       </c>
       <c r="AA36" s="11">
-        <f t="shared" ref="AA36:AA37" si="18">100/J36</f>
+        <f t="shared" ref="AA36:AA37" si="19">100/J36</f>
         <v>7.5757575757575761</v>
       </c>
       <c r="AB36" s="11">
-        <f t="shared" ref="AB36" si="19">100/K36</f>
+        <f t="shared" ref="AB36" si="20">100/K36</f>
         <v>2.2573363431151243</v>
       </c>
       <c r="AC36" s="12">
-        <f t="shared" ref="AC36:AC37" si="20">100/L36</f>
+        <f t="shared" ref="AC36:AD37" si="21">100/L36</f>
         <v>0.43103448275862066</v>
       </c>
-      <c r="AD36" s="11"/>
+      <c r="AD36" s="11">
+        <f t="shared" si="21"/>
+        <v>1.1441647597254003</v>
+      </c>
       <c r="AE36" s="11"/>
       <c r="AF36" s="11"/>
     </row>
-    <row r="37" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>7</v>
       </c>
@@ -1944,12 +2011,22 @@
       <c r="AA37" s="11"/>
       <c r="AB37" s="11"/>
       <c r="AC37" s="11">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>5.7670126874279122</v>
       </c>
       <c r="AD37" s="11"/>
       <c r="AE37" s="11"/>
       <c r="AF37" s="11"/>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update summary data and add csv version
</commit_message>
<xml_diff>
--- a/summary_data/gftp_summary.xlsx
+++ b/summary_data/gftp_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isfiligoi/github/tnrp-net-tests/summary_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98022C1-A8F7-B14F-AD71-436507EA3EC0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A22213C-CAF0-3741-A241-9DCB62DBDCA7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="-26640" windowWidth="47120" windowHeight="24500" xr2:uid="{F871B44F-434F-FB4B-AC1F-99327B90C475}"/>
   </bookViews>
@@ -517,7 +517,7 @@
   <dimension ref="A1:AF44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA43" sqref="AA43"/>
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1026,7 +1026,7 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3">
-        <v>7.4</v>
+        <v>7.9</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3">
@@ -1059,7 +1059,7 @@
       <c r="AB11" s="4"/>
       <c r="AC11" s="14">
         <f>100/L11</f>
-        <v>13.513513513513512</v>
+        <v>12.658227848101266</v>
       </c>
       <c r="AD11" s="4"/>
       <c r="AE11" s="4">
@@ -1218,8 +1218,12 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
+      <c r="N19" s="5">
+        <v>95.2</v>
+      </c>
+      <c r="O19" s="5">
+        <v>122</v>
+      </c>
       <c r="S19" t="str">
         <f>B19</f>
         <v>AWS EU C1</v>
@@ -1229,7 +1233,7 @@
         <v>1.893939393939394</v>
       </c>
       <c r="U19" s="13">
-        <f t="shared" ref="U19:V21" si="0">100/D19</f>
+        <f t="shared" ref="U19:V23" si="0">100/D19</f>
         <v>30.3951367781155</v>
       </c>
       <c r="V19" s="5"/>
@@ -1244,8 +1248,14 @@
       <c r="AB19" s="5"/>
       <c r="AC19" s="5"/>
       <c r="AD19" s="5"/>
-      <c r="AE19" s="5"/>
-      <c r="AF19" s="5"/>
+      <c r="AE19" s="6">
+        <f t="shared" ref="AE19:AF19" si="2">100/N19</f>
+        <v>1.0504201680672269</v>
+      </c>
+      <c r="AF19" s="6">
+        <f t="shared" si="2"/>
+        <v>0.81967213114754101</v>
+      </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
@@ -1265,7 +1275,9 @@
         <v>13.9</v>
       </c>
       <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="I20" s="5">
+        <v>12.5</v>
+      </c>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
@@ -1292,16 +1304,19 @@
         <v>3.1446540880503142</v>
       </c>
       <c r="X20" s="6">
-        <f t="shared" ref="X20:X23" si="2">100/G20</f>
+        <f t="shared" ref="X20:X23" si="3">100/G20</f>
         <v>7.1942446043165464</v>
       </c>
       <c r="Y20" s="6"/>
-      <c r="Z20" s="6"/>
+      <c r="Z20" s="6">
+        <f t="shared" ref="Z20:AA23" si="4">100/I20</f>
+        <v>8</v>
+      </c>
       <c r="AA20" s="6"/>
       <c r="AB20" s="6"/>
       <c r="AC20" s="6"/>
       <c r="AD20" s="6">
-        <f t="shared" ref="AC20:AD24" si="3">100/M20</f>
+        <f t="shared" ref="AC20:AF24" si="5">100/M20</f>
         <v>4.2553191489361701</v>
       </c>
       <c r="AE20" s="6"/>
@@ -1343,14 +1358,14 @@
         <v>NewYork</v>
       </c>
       <c r="T21" s="6">
-        <f t="shared" ref="T21" si="4">100/C21</f>
+        <f t="shared" ref="T21" si="6">100/C21</f>
         <v>1.0834236186348862</v>
       </c>
       <c r="U21" s="6">
         <f t="shared" si="0"/>
         <v>1.0893246187363834</v>
       </c>
-      <c r="V21" s="11">
+      <c r="V21" s="6">
         <f t="shared" si="0"/>
         <v>3.4482758620689653</v>
       </c>
@@ -1359,18 +1374,18 @@
         <v>10.309278350515465</v>
       </c>
       <c r="X21" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.698630136986301</v>
       </c>
       <c r="Y21" s="6"/>
       <c r="Z21" s="6"/>
       <c r="AA21" s="6">
-        <f t="shared" ref="AA21:AA23" si="5">100/J21</f>
+        <f t="shared" si="4"/>
         <v>1.0718113612004287</v>
       </c>
       <c r="AB21" s="6"/>
       <c r="AC21" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2.7700831024930745</v>
       </c>
       <c r="AD21" s="6"/>
@@ -1385,7 +1400,7 @@
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5">
-        <v>16.7</v>
+        <v>3.32</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -1403,9 +1418,9 @@
       <c r="T22" s="6"/>
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
-      <c r="W22" s="6">
+      <c r="W22" s="13">
         <f t="shared" si="1"/>
-        <v>5.9880239520958085</v>
+        <v>30.120481927710845</v>
       </c>
       <c r="X22" s="6"/>
       <c r="Y22" s="6"/>
@@ -1448,16 +1463,20 @@
       <c r="M23" s="5">
         <v>50.8</v>
       </c>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
+      <c r="N23" s="5">
+        <v>61.5</v>
+      </c>
+      <c r="O23" s="5">
+        <v>74.5</v>
+      </c>
       <c r="S23" t="str">
         <f>B23</f>
         <v>San Diego</v>
       </c>
       <c r="T23" s="6"/>
       <c r="U23" s="6"/>
-      <c r="V23" s="11">
-        <f t="shared" ref="V23" si="6">100/E23</f>
+      <c r="V23" s="6">
+        <f t="shared" si="0"/>
         <v>4.6296296296296298</v>
       </c>
       <c r="W23" s="6">
@@ -1465,7 +1484,7 @@
         <v>3.9215686274509802</v>
       </c>
       <c r="X23" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.7719298245614024</v>
       </c>
       <c r="Y23" s="6"/>
@@ -1474,7 +1493,7 @@
         <v>43.478260869565219</v>
       </c>
       <c r="AA23" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.9285714285714288</v>
       </c>
       <c r="AB23" s="6">
@@ -1482,15 +1501,21 @@
         <v>6.1349693251533743</v>
       </c>
       <c r="AC23" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>7.8125</v>
       </c>
       <c r="AD23" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.9685039370078741</v>
       </c>
-      <c r="AE23" s="6"/>
-      <c r="AF23" s="6"/>
+      <c r="AE23" s="6">
+        <f t="shared" si="5"/>
+        <v>1.6260162601626016</v>
+      </c>
+      <c r="AF23" s="6">
+        <f t="shared" si="5"/>
+        <v>1.3422818791946309</v>
+      </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
@@ -1508,11 +1533,15 @@
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5">
-        <v>16.7</v>
+        <v>3.3</v>
       </c>
       <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
+      <c r="N24" s="5">
+        <v>55.4</v>
+      </c>
+      <c r="O24" s="5">
+        <v>62.5</v>
+      </c>
       <c r="S24" t="str">
         <f>B24</f>
         <v>AWS US W2</v>
@@ -1529,13 +1558,19 @@
       <c r="Z24" s="6"/>
       <c r="AA24" s="6"/>
       <c r="AB24" s="6"/>
-      <c r="AC24" s="6">
-        <f t="shared" si="3"/>
-        <v>5.9880239520958085</v>
+      <c r="AC24" s="13">
+        <f t="shared" si="5"/>
+        <v>30.303030303030305</v>
       </c>
       <c r="AD24" s="6"/>
-      <c r="AE24" s="6"/>
-      <c r="AF24" s="6"/>
+      <c r="AE24" s="6">
+        <f t="shared" si="5"/>
+        <v>1.8050541516245489</v>
+      </c>
+      <c r="AF24" s="6">
+        <f t="shared" si="5"/>
+        <v>1.6</v>
+      </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.2">
       <c r="T25" s="2"/>
@@ -1699,8 +1734,12 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
       <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
+      <c r="N32" s="7">
+        <v>1810</v>
+      </c>
+      <c r="O32" s="7">
+        <v>1865</v>
+      </c>
       <c r="S32" t="str">
         <f>B32</f>
         <v>AWS EU C1</v>
@@ -1725,8 +1764,14 @@
       <c r="AB32" s="7"/>
       <c r="AC32" s="7"/>
       <c r="AD32" s="7"/>
-      <c r="AE32" s="7"/>
-      <c r="AF32" s="7"/>
+      <c r="AE32" s="12">
+        <f t="shared" ref="AE32:AF32" si="11">100/N32</f>
+        <v>5.5248618784530384E-2</v>
+      </c>
+      <c r="AF32" s="12">
+        <f t="shared" si="11"/>
+        <v>5.3619302949061663E-2</v>
+      </c>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
@@ -1746,7 +1791,9 @@
         <v>16.600000000000001</v>
       </c>
       <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
+      <c r="I33" s="7">
+        <v>194</v>
+      </c>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
       <c r="L33" s="7"/>
@@ -1773,16 +1820,19 @@
         <v>0.16583747927031509</v>
       </c>
       <c r="X33" s="11">
-        <f t="shared" ref="X33:X36" si="11">100/G33</f>
+        <f t="shared" ref="X33:X36" si="12">100/G33</f>
         <v>6.0240963855421681</v>
       </c>
       <c r="Y33" s="11"/>
-      <c r="Z33" s="11"/>
+      <c r="Z33" s="12">
+        <f t="shared" ref="Z33:AA36" si="13">100/I33</f>
+        <v>0.51546391752577314</v>
+      </c>
       <c r="AA33" s="11"/>
       <c r="AB33" s="11"/>
       <c r="AC33" s="11"/>
       <c r="AD33" s="11">
-        <f t="shared" ref="AD33" si="12">100/M33</f>
+        <f t="shared" ref="AD33" si="14">100/M33</f>
         <v>0.61349693251533743</v>
       </c>
       <c r="AE33" s="11"/>
@@ -1824,7 +1874,7 @@
         <v>NewYork</v>
       </c>
       <c r="T34" s="12">
-        <f t="shared" ref="T34" si="13">100/C34</f>
+        <f t="shared" ref="T34" si="15">100/C34</f>
         <v>0.14836795252225518</v>
       </c>
       <c r="U34" s="12">
@@ -1832,7 +1882,7 @@
         <v>0.17006802721088435</v>
       </c>
       <c r="V34" s="11">
-        <f t="shared" ref="V34:V36" si="14">100/E34</f>
+        <f t="shared" ref="V34:V36" si="16">100/E34</f>
         <v>1.2048192771084338</v>
       </c>
       <c r="W34" s="11">
@@ -1840,18 +1890,18 @@
         <v>2.2271714922048997</v>
       </c>
       <c r="X34" s="15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.989010989010989</v>
       </c>
       <c r="Y34" s="11"/>
       <c r="Z34" s="11"/>
       <c r="AA34" s="12">
-        <f t="shared" ref="AA34:AA36" si="15">100/J34</f>
+        <f t="shared" si="13"/>
         <v>0.4329004329004329</v>
       </c>
       <c r="AB34" s="11"/>
       <c r="AC34" s="12">
-        <f t="shared" ref="AC34:AC37" si="16">100/L34</f>
+        <f t="shared" ref="AC34:AC37" si="17">100/L34</f>
         <v>0.12376237623762376</v>
       </c>
       <c r="AD34" s="11"/>
@@ -1866,7 +1916,7 @@
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7">
-        <v>17.8</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
@@ -1886,7 +1936,7 @@
       <c r="V35" s="11"/>
       <c r="W35" s="11">
         <f t="shared" si="10"/>
-        <v>5.6179775280898872</v>
+        <v>6.2111801242236018</v>
       </c>
       <c r="X35" s="11"/>
       <c r="Y35" s="11"/>
@@ -1929,8 +1979,12 @@
       <c r="M36" s="7">
         <v>87.4</v>
       </c>
-      <c r="N36" s="7"/>
-      <c r="O36" s="7"/>
+      <c r="N36" s="7">
+        <v>950</v>
+      </c>
+      <c r="O36" s="7">
+        <v>995</v>
+      </c>
       <c r="S36" t="str">
         <f>B36</f>
         <v>San Diego</v>
@@ -1938,7 +1992,7 @@
       <c r="T36" s="11"/>
       <c r="U36" s="11"/>
       <c r="V36" s="11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>4.6296296296296298</v>
       </c>
       <c r="W36" s="12">
@@ -1946,32 +2000,38 @@
         <v>0.21598272138228941</v>
       </c>
       <c r="X36" s="11">
-        <f t="shared" ref="X36:X37" si="17">100/G36</f>
+        <f t="shared" ref="X36:X37" si="18">100/G36</f>
         <v>7.9365079365079367</v>
       </c>
       <c r="Y36" s="11"/>
       <c r="Z36" s="15">
-        <f t="shared" ref="Z36" si="18">100/I36</f>
+        <f t="shared" ref="Z36" si="19">100/I36</f>
         <v>17.361111111111111</v>
       </c>
       <c r="AA36" s="11">
-        <f t="shared" ref="AA36:AA37" si="19">100/J36</f>
+        <f t="shared" ref="AA36:AA37" si="20">100/J36</f>
         <v>7.5757575757575761</v>
       </c>
       <c r="AB36" s="11">
-        <f t="shared" ref="AB36" si="20">100/K36</f>
+        <f t="shared" ref="AB36" si="21">100/K36</f>
         <v>2.2573363431151243</v>
       </c>
       <c r="AC36" s="12">
-        <f t="shared" ref="AC36:AD37" si="21">100/L36</f>
+        <f t="shared" ref="AC36:AF37" si="22">100/L36</f>
         <v>0.43103448275862066</v>
       </c>
       <c r="AD36" s="11">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1.1441647597254003</v>
       </c>
-      <c r="AE36" s="11"/>
-      <c r="AF36" s="11"/>
+      <c r="AE36" s="12">
+        <f t="shared" si="22"/>
+        <v>0.10526315789473684</v>
+      </c>
+      <c r="AF36" s="12">
+        <f t="shared" si="22"/>
+        <v>0.10050251256281408</v>
+      </c>
     </row>
     <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
@@ -1981,7 +2041,7 @@
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7">
-        <v>33.799999999999997</v>
+        <v>514</v>
       </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
@@ -1989,11 +2049,15 @@
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
       <c r="L37" s="7">
-        <v>17.34</v>
+        <v>16.2</v>
       </c>
       <c r="M37" s="7"/>
-      <c r="N37" s="7"/>
-      <c r="O37" s="7"/>
+      <c r="N37" s="7">
+        <v>807</v>
+      </c>
+      <c r="O37" s="7">
+        <v>900</v>
+      </c>
       <c r="S37" t="str">
         <f>B37</f>
         <v>AWS US W2</v>
@@ -2001,9 +2065,9 @@
       <c r="T37" s="11"/>
       <c r="U37" s="11"/>
       <c r="V37" s="11"/>
-      <c r="W37" s="11">
+      <c r="W37" s="12">
         <f t="shared" si="10"/>
-        <v>2.9585798816568052</v>
+        <v>0.19455252918287938</v>
       </c>
       <c r="X37" s="11"/>
       <c r="Y37" s="11"/>
@@ -2011,12 +2075,18 @@
       <c r="AA37" s="11"/>
       <c r="AB37" s="11"/>
       <c r="AC37" s="11">
-        <f t="shared" si="21"/>
-        <v>5.7670126874279122</v>
+        <f t="shared" si="22"/>
+        <v>6.1728395061728394</v>
       </c>
       <c r="AD37" s="11"/>
-      <c r="AE37" s="11"/>
-      <c r="AF37" s="11"/>
+      <c r="AE37" s="12">
+        <f t="shared" si="22"/>
+        <v>0.12391573729863693</v>
+      </c>
+      <c r="AF37" s="12">
+        <f t="shared" si="22"/>
+        <v>0.1111111111111111</v>
+      </c>
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A43" t="s">

</xml_diff>

<commit_message>
Add Korea gftp tests
</commit_message>
<xml_diff>
--- a/summary_data/gftp_summary.xlsx
+++ b/summary_data/gftp_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isfiligoi/github/tnrp-net-tests/summary_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A22213C-CAF0-3741-A241-9DCB62DBDCA7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7492335-CA4B-5445-914B-54A9EFD37A31}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="-26640" windowWidth="47120" windowHeight="24500" xr2:uid="{F871B44F-434F-FB4B-AC1F-99327B90C475}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" xr2:uid="{F871B44F-434F-FB4B-AC1F-99327B90C475}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="23">
   <si>
     <t>Server</t>
   </si>
@@ -514,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AE2A42-D91B-564A-AB68-339151ECBD6D}">
-  <dimension ref="A1:AF44"/>
+  <dimension ref="A1:AF46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="K4" workbookViewId="0">
+      <selection activeCell="AE40" sqref="AE40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -599,55 +599,55 @@
         <v>Client</v>
       </c>
       <c r="T5" t="str">
-        <f>C5</f>
+        <f t="shared" ref="T5:AF5" si="0">C5</f>
         <v>AWS EU W1</v>
       </c>
       <c r="U5" t="str">
-        <f>D5</f>
+        <f t="shared" si="0"/>
         <v>AWS EU C1</v>
       </c>
       <c r="V5" t="str">
-        <f>E5</f>
+        <f t="shared" si="0"/>
         <v>Amsterdam</v>
       </c>
       <c r="W5" t="str">
-        <f>F5</f>
+        <f t="shared" si="0"/>
         <v>AWS US E1</v>
       </c>
       <c r="X5" t="str">
-        <f>G5</f>
+        <f t="shared" si="0"/>
         <v>Chicago</v>
       </c>
       <c r="Y5" t="str">
-        <f>H5</f>
+        <f t="shared" si="0"/>
         <v>Kansas</v>
       </c>
       <c r="Z5" t="str">
-        <f>I5</f>
+        <f t="shared" si="0"/>
         <v>San Diego</v>
       </c>
       <c r="AA5" t="str">
-        <f>J5</f>
+        <f t="shared" si="0"/>
         <v>GCP US W1</v>
       </c>
       <c r="AB5" t="str">
-        <f>K5</f>
+        <f t="shared" si="0"/>
         <v>Azure US W1</v>
       </c>
       <c r="AC5" t="str">
-        <f>L5</f>
+        <f t="shared" si="0"/>
         <v>AWS US W2</v>
       </c>
       <c r="AD5" t="str">
-        <f>M5</f>
+        <f t="shared" si="0"/>
         <v>Korea</v>
       </c>
       <c r="AE5" t="str">
-        <f>N5</f>
+        <f t="shared" si="0"/>
         <v>AWS Korea</v>
       </c>
       <c r="AF5" t="str">
-        <f>O5</f>
+        <f t="shared" si="0"/>
         <v>AWS Australia</v>
       </c>
     </row>
@@ -679,20 +679,20 @@
         <v>27.1</v>
       </c>
       <c r="S6" t="str">
-        <f>B6</f>
+        <f t="shared" ref="S6:S12" si="1">B6</f>
         <v>AWS EU C1</v>
       </c>
       <c r="T6" s="4">
-        <f>100/C6</f>
+        <f t="shared" ref="T6:U9" si="2">100/C6</f>
         <v>5.7471264367816097</v>
       </c>
       <c r="U6" s="14">
-        <f>100/D6</f>
+        <f t="shared" si="2"/>
         <v>13.333333333333334</v>
       </c>
       <c r="V6" s="3"/>
       <c r="W6" s="4">
-        <f>100/F6</f>
+        <f t="shared" ref="W6:W11" si="3">100/F6</f>
         <v>5.1020408163265305</v>
       </c>
       <c r="X6" s="3"/>
@@ -741,20 +741,20 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="S7" t="str">
-        <f>B7</f>
+        <f t="shared" si="1"/>
         <v>Amsterdam</v>
       </c>
       <c r="T7" s="4">
-        <f>100/C7</f>
+        <f t="shared" si="2"/>
         <v>9.1743119266055047</v>
       </c>
       <c r="U7" s="14">
-        <f>100/D7</f>
+        <f t="shared" si="2"/>
         <v>10.526315789473685</v>
       </c>
       <c r="V7" s="3"/>
       <c r="W7" s="4">
-        <f>100/F7</f>
+        <f t="shared" si="3"/>
         <v>7.8125</v>
       </c>
       <c r="X7" s="4">
@@ -812,15 +812,15 @@
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="S8" t="str">
-        <f>B8</f>
+        <f t="shared" si="1"/>
         <v>NewYork</v>
       </c>
       <c r="T8" s="4">
-        <f>100/C8</f>
+        <f t="shared" si="2"/>
         <v>1.0964912280701753</v>
       </c>
       <c r="U8" s="4">
-        <f>100/D8</f>
+        <f t="shared" si="2"/>
         <v>1.1325028312570782</v>
       </c>
       <c r="V8" s="4">
@@ -828,7 +828,7 @@
         <v>5.5865921787709505</v>
       </c>
       <c r="W8" s="14">
-        <f>100/F8</f>
+        <f t="shared" si="3"/>
         <v>10.526315789473685</v>
       </c>
       <c r="X8" s="14">
@@ -884,20 +884,20 @@
         <v>21.5</v>
       </c>
       <c r="S9" t="str">
-        <f>B9</f>
+        <f t="shared" si="1"/>
         <v>AWS US E1</v>
       </c>
       <c r="T9" s="4">
-        <f>100/C9</f>
+        <f t="shared" si="2"/>
         <v>5.2083333333333339</v>
       </c>
       <c r="U9" s="4">
-        <f>100/D9</f>
+        <f t="shared" si="2"/>
         <v>5.2356020942408374</v>
       </c>
       <c r="V9" s="4"/>
       <c r="W9" s="14">
-        <f>100/F9</f>
+        <f t="shared" si="3"/>
         <v>14.084507042253522</v>
       </c>
       <c r="X9" s="4"/>
@@ -908,11 +908,11 @@
       <c r="AC9" s="4"/>
       <c r="AD9" s="4"/>
       <c r="AE9" s="4">
-        <f>100/N9</f>
+        <f t="shared" ref="AE9:AF11" si="4">100/N9</f>
         <v>4.8780487804878048</v>
       </c>
       <c r="AF9" s="4">
-        <f>100/O9</f>
+        <f t="shared" si="4"/>
         <v>4.6511627906976747</v>
       </c>
     </row>
@@ -956,7 +956,7 @@
         <v>43.5</v>
       </c>
       <c r="S10" t="str">
-        <f>B10</f>
+        <f t="shared" si="1"/>
         <v>San Diego</v>
       </c>
       <c r="T10" s="4"/>
@@ -966,43 +966,43 @@
         <v>6.25</v>
       </c>
       <c r="W10" s="4">
-        <f>100/F10</f>
+        <f t="shared" si="3"/>
         <v>8.4033613445378155</v>
       </c>
       <c r="X10" s="4">
-        <f>100/G10</f>
+        <f t="shared" ref="X10:AD10" si="5">100/G10</f>
         <v>8.8495575221238933</v>
       </c>
       <c r="Y10" s="14">
-        <f>100/H10</f>
+        <f t="shared" si="5"/>
         <v>12.048192771084336</v>
       </c>
       <c r="Z10" s="14">
-        <f>100/I10</f>
+        <f t="shared" si="5"/>
         <v>12.987012987012987</v>
       </c>
       <c r="AA10" s="4">
-        <f>100/J10</f>
+        <f t="shared" si="5"/>
         <v>7.7519379844961236</v>
       </c>
       <c r="AB10" s="14">
-        <f>100/K10</f>
+        <f t="shared" si="5"/>
         <v>11.111111111111111</v>
       </c>
       <c r="AC10" s="4">
-        <f>100/L10</f>
+        <f t="shared" si="5"/>
         <v>9.2592592592592595</v>
       </c>
       <c r="AD10" s="4">
-        <f>100/M10</f>
+        <f t="shared" si="5"/>
         <v>6.9930069930069925</v>
       </c>
       <c r="AE10" s="4">
-        <f>100/N10</f>
+        <f t="shared" si="4"/>
         <v>5.3191489361702127</v>
       </c>
       <c r="AF10" s="4">
-        <f>100/O10</f>
+        <f t="shared" si="4"/>
         <v>2.2988505747126435</v>
       </c>
     </row>
@@ -1036,7 +1036,7 @@
         <v>21.7</v>
       </c>
       <c r="S11" t="str">
-        <f>B11</f>
+        <f t="shared" si="1"/>
         <v>AWS US W2</v>
       </c>
       <c r="T11" s="4">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="V11" s="4"/>
       <c r="W11" s="4">
-        <f>100/F11</f>
+        <f t="shared" si="3"/>
         <v>5.4347826086956523</v>
       </c>
       <c r="X11" s="4"/>
@@ -1063,1038 +1063,1148 @@
       </c>
       <c r="AD11" s="4"/>
       <c r="AE11" s="4">
-        <f>100/N11</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="AF11" s="4">
-        <f>100/O11</f>
+        <f t="shared" si="4"/>
         <v>4.6082949308755765</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3">
+        <v>20.6</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="O12" s="3"/>
+      <c r="S12" t="str">
+        <f t="shared" si="1"/>
+        <v>Korea</v>
+      </c>
+      <c r="T12" s="4"/>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4">
+        <f>100/I12</f>
+        <v>4.8543689320388346</v>
+      </c>
+      <c r="AA12" s="4"/>
+      <c r="AB12" s="4"/>
+      <c r="AC12" s="14"/>
+      <c r="AD12" s="4"/>
+      <c r="AE12" s="4">
+        <f>100/N12</f>
+        <v>10.309278350515465</v>
+      </c>
+      <c r="AF12" s="4"/>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="R14" s="9" t="str">
-        <f>A14</f>
+      <c r="R15" s="9" t="str">
+        <f>A15</f>
         <v>GridFTP tests - single threaded, multiple processes</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>0</v>
       </c>
-      <c r="S17" t="str">
-        <f>B17</f>
+      <c r="S18" t="str">
+        <f>B18</f>
         <v>Server</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>15</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>2</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
         <v>3</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" t="s">
         <v>8</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" t="s">
         <v>4</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H19" t="s">
         <v>5</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I19" t="s">
         <v>6</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J19" t="s">
         <v>9</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K19" t="s">
         <v>10</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L19" t="s">
         <v>7</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N19" t="s">
         <v>11</v>
       </c>
-      <c r="O18" t="s">
+      <c r="O19" t="s">
         <v>12</v>
       </c>
-      <c r="R18" t="str">
-        <f>A18</f>
+      <c r="R19" t="str">
+        <f>A19</f>
         <v>Client</v>
       </c>
-      <c r="T18" t="str">
-        <f>C18</f>
+      <c r="T19" t="str">
+        <f t="shared" ref="T19:AF19" si="6">C19</f>
         <v>AWS EU W1</v>
       </c>
-      <c r="U18" t="str">
-        <f>D18</f>
+      <c r="U19" t="str">
+        <f t="shared" si="6"/>
         <v>AWS EU C1</v>
       </c>
-      <c r="V18" t="str">
-        <f>E18</f>
+      <c r="V19" t="str">
+        <f t="shared" si="6"/>
         <v>Amsterdam</v>
       </c>
-      <c r="W18" t="str">
-        <f>F18</f>
+      <c r="W19" t="str">
+        <f t="shared" si="6"/>
         <v>AWS US E1</v>
       </c>
-      <c r="X18" t="str">
-        <f>G18</f>
+      <c r="X19" t="str">
+        <f t="shared" si="6"/>
         <v>Chicago</v>
       </c>
-      <c r="Y18" t="str">
-        <f>H18</f>
+      <c r="Y19" t="str">
+        <f t="shared" si="6"/>
         <v>Kansas</v>
       </c>
-      <c r="Z18" t="str">
-        <f>I18</f>
+      <c r="Z19" t="str">
+        <f t="shared" si="6"/>
         <v>San Diego</v>
       </c>
-      <c r="AA18" t="str">
-        <f>J18</f>
+      <c r="AA19" t="str">
+        <f t="shared" si="6"/>
         <v>GCP US W1</v>
       </c>
-      <c r="AB18" t="str">
-        <f>K18</f>
+      <c r="AB19" t="str">
+        <f t="shared" si="6"/>
         <v>Azure US W1</v>
       </c>
-      <c r="AC18" t="str">
-        <f>L18</f>
+      <c r="AC19" t="str">
+        <f t="shared" si="6"/>
         <v>AWS US W2</v>
       </c>
-      <c r="AD18" t="str">
-        <f>M18</f>
+      <c r="AD19" t="str">
+        <f t="shared" si="6"/>
         <v>Korea</v>
       </c>
-      <c r="AE18" t="str">
-        <f>N18</f>
+      <c r="AE19" t="str">
+        <f t="shared" si="6"/>
         <v>AWS Korea</v>
       </c>
-      <c r="AF18" t="str">
-        <f>O18</f>
+      <c r="AF19" t="str">
+        <f t="shared" si="6"/>
         <v>AWS Australia</v>
-      </c>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="5">
-        <v>52.8</v>
-      </c>
-      <c r="D19" s="5">
-        <v>3.29</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5">
-        <v>52.7</v>
-      </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5">
-        <v>95.2</v>
-      </c>
-      <c r="O19" s="5">
-        <v>122</v>
-      </c>
-      <c r="S19" t="str">
-        <f>B19</f>
-        <v>AWS EU C1</v>
-      </c>
-      <c r="T19" s="6">
-        <f>100/C19</f>
-        <v>1.893939393939394</v>
-      </c>
-      <c r="U19" s="13">
-        <f t="shared" ref="U19:V23" si="0">100/D19</f>
-        <v>30.3951367781155</v>
-      </c>
-      <c r="V19" s="5"/>
-      <c r="W19" s="6">
-        <f t="shared" ref="W19:W24" si="1">100/F19</f>
-        <v>1.8975332068311195</v>
-      </c>
-      <c r="X19" s="5"/>
-      <c r="Y19" s="5"/>
-      <c r="Z19" s="5"/>
-      <c r="AA19" s="5"/>
-      <c r="AB19" s="5"/>
-      <c r="AC19" s="5"/>
-      <c r="AD19" s="5"/>
-      <c r="AE19" s="6">
-        <f t="shared" ref="AE19:AF19" si="2">100/N19</f>
-        <v>1.0504201680672269</v>
-      </c>
-      <c r="AF19" s="6">
-        <f t="shared" si="2"/>
-        <v>0.81967213114754101</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20" s="5">
-        <v>10.7</v>
+        <v>52.8</v>
       </c>
       <c r="D20" s="5">
-        <v>10.5</v>
+        <v>3.29</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5">
-        <v>31.8</v>
-      </c>
-      <c r="G20" s="5">
-        <v>13.9</v>
-      </c>
+        <v>52.7</v>
+      </c>
+      <c r="G20" s="5"/>
       <c r="H20" s="5"/>
-      <c r="I20" s="5">
-        <v>12.5</v>
-      </c>
+      <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
-      <c r="M20" s="5">
-        <v>23.5</v>
-      </c>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5">
+        <v>95.2</v>
+      </c>
+      <c r="O20" s="5">
+        <v>122</v>
+      </c>
       <c r="S20" t="str">
-        <f>B20</f>
-        <v>Amsterdam</v>
+        <f t="shared" ref="S20:S26" si="7">B20</f>
+        <v>AWS EU C1</v>
       </c>
       <c r="T20" s="6">
         <f>100/C20</f>
-        <v>9.3457943925233646</v>
-      </c>
-      <c r="U20" s="6">
-        <f t="shared" si="0"/>
-        <v>9.5238095238095237</v>
-      </c>
-      <c r="V20" s="6"/>
+        <v>1.893939393939394</v>
+      </c>
+      <c r="U20" s="13">
+        <f t="shared" ref="U20:V24" si="8">100/D20</f>
+        <v>30.3951367781155</v>
+      </c>
+      <c r="V20" s="5"/>
       <c r="W20" s="6">
-        <f t="shared" si="1"/>
-        <v>3.1446540880503142</v>
-      </c>
-      <c r="X20" s="6">
-        <f t="shared" ref="X20:X23" si="3">100/G20</f>
-        <v>7.1942446043165464</v>
-      </c>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="6">
-        <f t="shared" ref="Z20:AA23" si="4">100/I20</f>
-        <v>8</v>
-      </c>
-      <c r="AA20" s="6"/>
-      <c r="AB20" s="6"/>
-      <c r="AC20" s="6"/>
-      <c r="AD20" s="6">
-        <f t="shared" ref="AC20:AF24" si="5">100/M20</f>
-        <v>4.2553191489361701</v>
-      </c>
-      <c r="AE20" s="6"/>
-      <c r="AF20" s="6"/>
+        <f t="shared" ref="W20:W25" si="9">100/F20</f>
+        <v>1.8975332068311195</v>
+      </c>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="5"/>
+      <c r="AC20" s="5"/>
+      <c r="AD20" s="5"/>
+      <c r="AE20" s="6">
+        <f t="shared" ref="AE20:AF20" si="10">100/N20</f>
+        <v>1.0504201680672269</v>
+      </c>
+      <c r="AF20" s="6">
+        <f t="shared" si="10"/>
+        <v>0.81967213114754101</v>
+      </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C21" s="5">
-        <v>92.3</v>
+        <v>10.7</v>
       </c>
       <c r="D21" s="5">
-        <v>91.8</v>
-      </c>
-      <c r="E21" s="5">
-        <v>29</v>
-      </c>
+        <v>10.5</v>
+      </c>
+      <c r="E21" s="5"/>
       <c r="F21" s="5">
-        <v>9.6999999999999993</v>
+        <v>31.8</v>
       </c>
       <c r="G21" s="5">
-        <v>7.3</v>
+        <v>13.9</v>
       </c>
       <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5">
-        <v>93.3</v>
-      </c>
+      <c r="I21" s="5">
+        <v>12.5</v>
+      </c>
+      <c r="J21" s="5"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="5">
-        <v>36.1</v>
-      </c>
-      <c r="M21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5">
+        <v>23.5</v>
+      </c>
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="S21" t="str">
-        <f>B21</f>
-        <v>NewYork</v>
+        <f t="shared" si="7"/>
+        <v>Amsterdam</v>
       </c>
       <c r="T21" s="6">
-        <f t="shared" ref="T21" si="6">100/C21</f>
-        <v>1.0834236186348862</v>
+        <f>100/C21</f>
+        <v>9.3457943925233646</v>
       </c>
       <c r="U21" s="6">
-        <f t="shared" si="0"/>
-        <v>1.0893246187363834</v>
-      </c>
-      <c r="V21" s="6">
-        <f t="shared" si="0"/>
-        <v>3.4482758620689653</v>
-      </c>
-      <c r="W21" s="13">
-        <f t="shared" si="1"/>
-        <v>10.309278350515465</v>
-      </c>
-      <c r="X21" s="13">
-        <f t="shared" si="3"/>
-        <v>13.698630136986301</v>
+        <f t="shared" si="8"/>
+        <v>9.5238095238095237</v>
+      </c>
+      <c r="V21" s="6"/>
+      <c r="W21" s="6">
+        <f t="shared" si="9"/>
+        <v>3.1446540880503142</v>
+      </c>
+      <c r="X21" s="6">
+        <f t="shared" ref="X21:X24" si="11">100/G21</f>
+        <v>7.1942446043165464</v>
       </c>
       <c r="Y21" s="6"/>
-      <c r="Z21" s="6"/>
-      <c r="AA21" s="6">
-        <f t="shared" si="4"/>
-        <v>1.0718113612004287</v>
-      </c>
+      <c r="Z21" s="6">
+        <f t="shared" ref="Z21:AA26" si="12">100/I21</f>
+        <v>8</v>
+      </c>
+      <c r="AA21" s="6"/>
       <c r="AB21" s="6"/>
-      <c r="AC21" s="6">
-        <f t="shared" si="5"/>
-        <v>2.7700831024930745</v>
-      </c>
-      <c r="AD21" s="6"/>
+      <c r="AC21" s="6"/>
+      <c r="AD21" s="6">
+        <f t="shared" ref="AC21:AF25" si="13">100/M21</f>
+        <v>4.2553191489361701</v>
+      </c>
       <c r="AE21" s="6"/>
       <c r="AF21" s="6"/>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+        <v>13</v>
+      </c>
+      <c r="C22" s="5">
+        <v>92.3</v>
+      </c>
+      <c r="D22" s="5">
+        <v>91.8</v>
+      </c>
+      <c r="E22" s="5">
+        <v>29</v>
+      </c>
       <c r="F22" s="5">
-        <v>3.32</v>
-      </c>
-      <c r="G22" s="5"/>
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="G22" s="5">
+        <v>7.3</v>
+      </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
+      <c r="J22" s="5">
+        <v>93.3</v>
+      </c>
       <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
+      <c r="L22" s="5">
+        <v>36.1</v>
+      </c>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="S22" t="str">
-        <f>B22</f>
-        <v>AWS US E1</v>
-      </c>
-      <c r="T22" s="6"/>
-      <c r="U22" s="6"/>
-      <c r="V22" s="6"/>
+        <f t="shared" si="7"/>
+        <v>NewYork</v>
+      </c>
+      <c r="T22" s="6">
+        <f t="shared" ref="T22" si="14">100/C22</f>
+        <v>1.0834236186348862</v>
+      </c>
+      <c r="U22" s="6">
+        <f t="shared" si="8"/>
+        <v>1.0893246187363834</v>
+      </c>
+      <c r="V22" s="6">
+        <f t="shared" si="8"/>
+        <v>3.4482758620689653</v>
+      </c>
       <c r="W22" s="13">
-        <f t="shared" si="1"/>
-        <v>30.120481927710845</v>
-      </c>
-      <c r="X22" s="6"/>
+        <f t="shared" si="9"/>
+        <v>10.309278350515465</v>
+      </c>
+      <c r="X22" s="13">
+        <f t="shared" si="11"/>
+        <v>13.698630136986301</v>
+      </c>
       <c r="Y22" s="6"/>
       <c r="Z22" s="6"/>
-      <c r="AA22" s="6"/>
+      <c r="AA22" s="6">
+        <f t="shared" si="12"/>
+        <v>1.0718113612004287</v>
+      </c>
       <c r="AB22" s="6"/>
-      <c r="AC22" s="6"/>
+      <c r="AC22" s="6">
+        <f t="shared" si="13"/>
+        <v>2.7700831024930745</v>
+      </c>
       <c r="AD22" s="6"/>
       <c r="AE22" s="6"/>
       <c r="AF22" s="6"/>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="5">
-        <v>21.6</v>
-      </c>
+      <c r="E23" s="5"/>
       <c r="F23" s="5">
-        <v>25.5</v>
-      </c>
-      <c r="G23" s="5">
-        <v>11.4</v>
-      </c>
+        <v>3.32</v>
+      </c>
+      <c r="G23" s="5"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="5">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="J23" s="5">
-        <v>11.2</v>
-      </c>
-      <c r="K23" s="5">
-        <v>16.3</v>
-      </c>
-      <c r="L23" s="5">
-        <v>12.8</v>
-      </c>
-      <c r="M23" s="5">
-        <v>50.8</v>
-      </c>
-      <c r="N23" s="5">
-        <v>61.5</v>
-      </c>
-      <c r="O23" s="5">
-        <v>74.5</v>
-      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
       <c r="S23" t="str">
-        <f>B23</f>
-        <v>San Diego</v>
+        <f t="shared" si="7"/>
+        <v>AWS US E1</v>
       </c>
       <c r="T23" s="6"/>
       <c r="U23" s="6"/>
-      <c r="V23" s="6">
-        <f t="shared" si="0"/>
-        <v>4.6296296296296298</v>
-      </c>
-      <c r="W23" s="6">
-        <f t="shared" si="1"/>
-        <v>3.9215686274509802</v>
-      </c>
-      <c r="X23" s="6">
-        <f t="shared" si="3"/>
-        <v>8.7719298245614024</v>
-      </c>
+      <c r="V23" s="6"/>
+      <c r="W23" s="13">
+        <f t="shared" si="9"/>
+        <v>30.120481927710845</v>
+      </c>
+      <c r="X23" s="6"/>
       <c r="Y23" s="6"/>
-      <c r="Z23" s="13">
-        <f t="shared" ref="Z23" si="7">100/I23</f>
-        <v>43.478260869565219</v>
-      </c>
-      <c r="AA23" s="6">
-        <f t="shared" si="4"/>
-        <v>8.9285714285714288</v>
-      </c>
-      <c r="AB23" s="6">
-        <f t="shared" ref="AB23" si="8">100/K23</f>
-        <v>6.1349693251533743</v>
-      </c>
-      <c r="AC23" s="6">
-        <f t="shared" si="5"/>
-        <v>7.8125</v>
-      </c>
-      <c r="AD23" s="6">
-        <f t="shared" si="5"/>
-        <v>1.9685039370078741</v>
-      </c>
-      <c r="AE23" s="6">
-        <f t="shared" si="5"/>
-        <v>1.6260162601626016</v>
-      </c>
-      <c r="AF23" s="6">
-        <f t="shared" si="5"/>
-        <v>1.3422818791946309</v>
-      </c>
+      <c r="Z23" s="6"/>
+      <c r="AA23" s="6"/>
+      <c r="AB23" s="6"/>
+      <c r="AC23" s="6"/>
+      <c r="AD23" s="6"/>
+      <c r="AE23" s="6"/>
+      <c r="AF23" s="6"/>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="E24" s="5">
+        <v>21.6</v>
+      </c>
       <c r="F24" s="5">
-        <v>54.4</v>
-      </c>
-      <c r="G24" s="5"/>
+        <v>25.5</v>
+      </c>
+      <c r="G24" s="5">
+        <v>11.4</v>
+      </c>
       <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
+      <c r="I24" s="5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J24" s="5">
+        <v>11.2</v>
+      </c>
+      <c r="K24" s="5">
+        <v>16.3</v>
+      </c>
       <c r="L24" s="5">
-        <v>3.3</v>
-      </c>
-      <c r="M24" s="5"/>
+        <v>12.8</v>
+      </c>
+      <c r="M24" s="5">
+        <v>50.8</v>
+      </c>
       <c r="N24" s="5">
-        <v>55.4</v>
+        <v>61.5</v>
       </c>
       <c r="O24" s="5">
-        <v>62.5</v>
+        <v>74.5</v>
       </c>
       <c r="S24" t="str">
-        <f>B24</f>
-        <v>AWS US W2</v>
+        <f t="shared" si="7"/>
+        <v>San Diego</v>
       </c>
       <c r="T24" s="6"/>
       <c r="U24" s="6"/>
-      <c r="V24" s="6"/>
+      <c r="V24" s="6">
+        <f t="shared" si="8"/>
+        <v>4.6296296296296298</v>
+      </c>
       <c r="W24" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="9"/>
+        <v>3.9215686274509802</v>
+      </c>
+      <c r="X24" s="6">
+        <f t="shared" si="11"/>
+        <v>8.7719298245614024</v>
+      </c>
+      <c r="Y24" s="6"/>
+      <c r="Z24" s="13">
+        <f t="shared" ref="Z24" si="15">100/I24</f>
+        <v>43.478260869565219</v>
+      </c>
+      <c r="AA24" s="6">
+        <f t="shared" si="12"/>
+        <v>8.9285714285714288</v>
+      </c>
+      <c r="AB24" s="6">
+        <f t="shared" ref="AB24" si="16">100/K24</f>
+        <v>6.1349693251533743</v>
+      </c>
+      <c r="AC24" s="6">
+        <f t="shared" si="13"/>
+        <v>7.8125</v>
+      </c>
+      <c r="AD24" s="6">
+        <f t="shared" si="13"/>
+        <v>1.9685039370078741</v>
+      </c>
+      <c r="AE24" s="6">
+        <f t="shared" si="13"/>
+        <v>1.6260162601626016</v>
+      </c>
+      <c r="AF24" s="6">
+        <f t="shared" si="13"/>
+        <v>1.3422818791946309</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5">
+        <v>54.4</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5">
+        <v>3.3</v>
+      </c>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5">
+        <v>55.4</v>
+      </c>
+      <c r="O25" s="5">
+        <v>62.5</v>
+      </c>
+      <c r="S25" t="str">
+        <f t="shared" si="7"/>
+        <v>AWS US W2</v>
+      </c>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6">
+        <f t="shared" si="9"/>
         <v>1.8382352941176472</v>
       </c>
-      <c r="X24" s="6"/>
-      <c r="Y24" s="6"/>
-      <c r="Z24" s="6"/>
-      <c r="AA24" s="6"/>
-      <c r="AB24" s="6"/>
-      <c r="AC24" s="13">
-        <f t="shared" si="5"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6"/>
+      <c r="Z25" s="6"/>
+      <c r="AA25" s="6"/>
+      <c r="AB25" s="6"/>
+      <c r="AC25" s="13">
+        <f t="shared" si="13"/>
         <v>30.303030303030305</v>
       </c>
-      <c r="AD24" s="6"/>
-      <c r="AE24" s="6">
-        <f t="shared" si="5"/>
+      <c r="AD25" s="6"/>
+      <c r="AE25" s="6">
+        <f t="shared" si="13"/>
         <v>1.8050541516245489</v>
       </c>
-      <c r="AF24" s="6">
-        <f t="shared" si="5"/>
+      <c r="AF25" s="6">
+        <f t="shared" si="13"/>
         <v>1.6</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="2"/>
-      <c r="W25" s="2"/>
-      <c r="X25" s="2"/>
-      <c r="Y25" s="2"/>
-      <c r="Z25" s="2"/>
-      <c r="AA25" s="2"/>
-      <c r="AB25" s="2"/>
-      <c r="AC25" s="2"/>
-      <c r="AD25" s="2"/>
-      <c r="AE25" s="2"/>
-      <c r="AF25" s="2"/>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5">
+        <v>18.3</v>
+      </c>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5">
+        <v>12.9</v>
+      </c>
+      <c r="O26" s="5"/>
+      <c r="S26" t="str">
+        <f t="shared" si="7"/>
+        <v>Korea</v>
+      </c>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="6"/>
+      <c r="X26" s="6"/>
+      <c r="Y26" s="6"/>
+      <c r="Z26" s="6">
+        <f t="shared" si="12"/>
+        <v>5.4644808743169397</v>
+      </c>
+      <c r="AA26" s="6"/>
+      <c r="AB26" s="6"/>
+      <c r="AC26" s="13"/>
+      <c r="AD26" s="6"/>
+      <c r="AE26" s="6"/>
+      <c r="AF26" s="6"/>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+      <c r="W27" s="2"/>
+      <c r="X27" s="2"/>
+      <c r="Y27" s="2"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
+      <c r="AD27" s="2"/>
+      <c r="AE27" s="2"/>
+      <c r="AF27" s="2"/>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="R27" s="8" t="str">
-        <f>A27</f>
+      <c r="R29" s="8" t="str">
+        <f>A29</f>
         <v>GridFTP tests - single threaded, single process</v>
-      </c>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="R29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>0</v>
-      </c>
-      <c r="S30" t="str">
-        <f>B30</f>
-        <v>Server</v>
       </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" t="s">
-        <v>3</v>
-      </c>
-      <c r="F31" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" t="s">
-        <v>4</v>
-      </c>
-      <c r="H31" t="s">
-        <v>5</v>
-      </c>
-      <c r="I31" t="s">
-        <v>6</v>
-      </c>
-      <c r="J31" t="s">
-        <v>9</v>
-      </c>
-      <c r="K31" t="s">
-        <v>10</v>
-      </c>
-      <c r="L31" t="s">
-        <v>7</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N31" t="s">
-        <v>11</v>
-      </c>
-      <c r="O31" t="s">
-        <v>12</v>
-      </c>
-      <c r="R31" t="str">
-        <f>A31</f>
-        <v>Client</v>
-      </c>
-      <c r="T31" t="str">
-        <f>C31</f>
-        <v>AWS EU W1</v>
-      </c>
-      <c r="U31" t="str">
-        <f>D31</f>
-        <v>AWS EU C1</v>
-      </c>
-      <c r="V31" t="str">
-        <f>E31</f>
-        <v>Amsterdam</v>
-      </c>
-      <c r="W31" t="str">
-        <f>F31</f>
-        <v>AWS US E1</v>
-      </c>
-      <c r="X31" t="str">
-        <f>G31</f>
-        <v>Chicago</v>
-      </c>
-      <c r="Y31" t="str">
-        <f>H31</f>
-        <v>Kansas</v>
-      </c>
-      <c r="Z31" t="str">
-        <f>I31</f>
-        <v>San Diego</v>
-      </c>
-      <c r="AA31" t="str">
-        <f>J31</f>
-        <v>GCP US W1</v>
-      </c>
-      <c r="AB31" t="str">
-        <f>K31</f>
-        <v>Azure US W1</v>
-      </c>
-      <c r="AC31" t="str">
-        <f>L31</f>
-        <v>AWS US W2</v>
-      </c>
-      <c r="AD31" t="str">
-        <f>M31</f>
-        <v>Korea</v>
-      </c>
-      <c r="AE31" t="str">
-        <f>N31</f>
-        <v>AWS Korea</v>
-      </c>
-      <c r="AF31" t="str">
-        <f>O31</f>
-        <v>AWS Australia</v>
+        <v>14</v>
+      </c>
+      <c r="R31" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" s="7">
-        <v>167</v>
-      </c>
-      <c r="D32" s="7">
-        <v>8.6</v>
-      </c>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7">
-        <v>566</v>
-      </c>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7">
-        <v>1810</v>
-      </c>
-      <c r="O32" s="7">
-        <v>1865</v>
+        <v>0</v>
       </c>
       <c r="S32" t="str">
         <f>B32</f>
+        <v>Server</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" t="s">
+        <v>4</v>
+      </c>
+      <c r="H33" t="s">
+        <v>5</v>
+      </c>
+      <c r="I33" t="s">
+        <v>6</v>
+      </c>
+      <c r="J33" t="s">
+        <v>9</v>
+      </c>
+      <c r="K33" t="s">
+        <v>10</v>
+      </c>
+      <c r="L33" t="s">
+        <v>7</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N33" t="s">
+        <v>11</v>
+      </c>
+      <c r="O33" t="s">
+        <v>12</v>
+      </c>
+      <c r="R33" t="str">
+        <f>A33</f>
+        <v>Client</v>
+      </c>
+      <c r="T33" t="str">
+        <f t="shared" ref="T33:AF33" si="17">C33</f>
+        <v>AWS EU W1</v>
+      </c>
+      <c r="U33" t="str">
+        <f t="shared" si="17"/>
         <v>AWS EU C1</v>
       </c>
-      <c r="T32" s="12">
-        <f>100/C32</f>
-        <v>0.59880239520958078</v>
-      </c>
-      <c r="U32" s="15">
-        <f t="shared" ref="U32:U34" si="9">100/D32</f>
-        <v>11.627906976744187</v>
-      </c>
-      <c r="V32" s="7"/>
-      <c r="W32" s="12">
-        <f t="shared" ref="W32:W37" si="10">100/F32</f>
-        <v>0.17667844522968199</v>
-      </c>
-      <c r="X32" s="7"/>
-      <c r="Y32" s="7"/>
-      <c r="Z32" s="7"/>
-      <c r="AA32" s="7"/>
-      <c r="AB32" s="7"/>
-      <c r="AC32" s="7"/>
-      <c r="AD32" s="7"/>
-      <c r="AE32" s="12">
-        <f t="shared" ref="AE32:AF32" si="11">100/N32</f>
-        <v>5.5248618784530384E-2</v>
-      </c>
-      <c r="AF32" s="12">
-        <f t="shared" si="11"/>
-        <v>5.3619302949061663E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" s="7">
-        <v>153</v>
-      </c>
-      <c r="D33" s="7">
-        <v>46.7</v>
-      </c>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7">
-        <v>603</v>
-      </c>
-      <c r="G33" s="7">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7">
-        <v>194</v>
-      </c>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7">
-        <v>163</v>
-      </c>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7"/>
-      <c r="S33" t="str">
-        <f>B33</f>
+      <c r="V33" t="str">
+        <f t="shared" si="17"/>
         <v>Amsterdam</v>
       </c>
-      <c r="T33" s="12">
-        <f>100/C33</f>
-        <v>0.65359477124183007</v>
-      </c>
-      <c r="U33" s="11">
-        <f t="shared" si="9"/>
-        <v>2.1413276231263381</v>
-      </c>
-      <c r="V33" s="11"/>
-      <c r="W33" s="12">
-        <f t="shared" si="10"/>
-        <v>0.16583747927031509</v>
-      </c>
-      <c r="X33" s="11">
-        <f t="shared" ref="X33:X36" si="12">100/G33</f>
-        <v>6.0240963855421681</v>
-      </c>
-      <c r="Y33" s="11"/>
-      <c r="Z33" s="12">
-        <f t="shared" ref="Z33:AA36" si="13">100/I33</f>
-        <v>0.51546391752577314</v>
-      </c>
-      <c r="AA33" s="11"/>
-      <c r="AB33" s="11"/>
-      <c r="AC33" s="11"/>
-      <c r="AD33" s="11">
-        <f t="shared" ref="AD33" si="14">100/M33</f>
-        <v>0.61349693251533743</v>
-      </c>
-      <c r="AE33" s="11"/>
-      <c r="AF33" s="11"/>
+      <c r="W33" t="str">
+        <f t="shared" si="17"/>
+        <v>AWS US E1</v>
+      </c>
+      <c r="X33" t="str">
+        <f t="shared" si="17"/>
+        <v>Chicago</v>
+      </c>
+      <c r="Y33" t="str">
+        <f t="shared" si="17"/>
+        <v>Kansas</v>
+      </c>
+      <c r="Z33" t="str">
+        <f t="shared" si="17"/>
+        <v>San Diego</v>
+      </c>
+      <c r="AA33" t="str">
+        <f t="shared" si="17"/>
+        <v>GCP US W1</v>
+      </c>
+      <c r="AB33" t="str">
+        <f t="shared" si="17"/>
+        <v>Azure US W1</v>
+      </c>
+      <c r="AC33" t="str">
+        <f t="shared" si="17"/>
+        <v>AWS US W2</v>
+      </c>
+      <c r="AD33" t="str">
+        <f t="shared" si="17"/>
+        <v>Korea</v>
+      </c>
+      <c r="AE33" t="str">
+        <f t="shared" si="17"/>
+        <v>AWS Korea</v>
+      </c>
+      <c r="AF33" t="str">
+        <f t="shared" si="17"/>
+        <v>AWS Australia</v>
+      </c>
     </row>
     <row r="34" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C34" s="7">
-        <v>674</v>
+        <v>167</v>
       </c>
       <c r="D34" s="7">
-        <v>588</v>
-      </c>
-      <c r="E34" s="7">
-        <v>83</v>
-      </c>
+        <v>8.6</v>
+      </c>
+      <c r="E34" s="7"/>
       <c r="F34" s="7">
-        <v>44.9</v>
-      </c>
-      <c r="G34" s="7">
-        <v>9.1</v>
-      </c>
+        <v>566</v>
+      </c>
+      <c r="G34" s="7"/>
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
-      <c r="J34" s="7">
-        <v>231</v>
-      </c>
+      <c r="J34" s="7"/>
       <c r="K34" s="7"/>
-      <c r="L34" s="7">
-        <v>808</v>
-      </c>
+      <c r="L34" s="7"/>
       <c r="M34" s="7"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="7"/>
+      <c r="N34" s="7">
+        <v>1810</v>
+      </c>
+      <c r="O34" s="7">
+        <v>1865</v>
+      </c>
       <c r="S34" t="str">
-        <f>B34</f>
-        <v>NewYork</v>
+        <f t="shared" ref="S34:S40" si="18">B34</f>
+        <v>AWS EU C1</v>
       </c>
       <c r="T34" s="12">
-        <f t="shared" ref="T34" si="15">100/C34</f>
-        <v>0.14836795252225518</v>
-      </c>
-      <c r="U34" s="12">
-        <f t="shared" si="9"/>
-        <v>0.17006802721088435</v>
-      </c>
-      <c r="V34" s="11">
-        <f t="shared" ref="V34:V36" si="16">100/E34</f>
-        <v>1.2048192771084338</v>
-      </c>
-      <c r="W34" s="11">
-        <f t="shared" si="10"/>
-        <v>2.2271714922048997</v>
-      </c>
-      <c r="X34" s="15">
-        <f t="shared" si="12"/>
-        <v>10.989010989010989</v>
-      </c>
-      <c r="Y34" s="11"/>
-      <c r="Z34" s="11"/>
-      <c r="AA34" s="12">
-        <f t="shared" si="13"/>
-        <v>0.4329004329004329</v>
-      </c>
-      <c r="AB34" s="11"/>
-      <c r="AC34" s="12">
-        <f t="shared" ref="AC34:AC37" si="17">100/L34</f>
-        <v>0.12376237623762376</v>
-      </c>
-      <c r="AD34" s="11"/>
-      <c r="AE34" s="11"/>
-      <c r="AF34" s="11"/>
+        <f>100/C34</f>
+        <v>0.59880239520958078</v>
+      </c>
+      <c r="U34" s="15">
+        <f t="shared" ref="U34:U36" si="19">100/D34</f>
+        <v>11.627906976744187</v>
+      </c>
+      <c r="V34" s="7"/>
+      <c r="W34" s="12">
+        <f t="shared" ref="W34:W39" si="20">100/F34</f>
+        <v>0.17667844522968199</v>
+      </c>
+      <c r="X34" s="7"/>
+      <c r="Y34" s="7"/>
+      <c r="Z34" s="7"/>
+      <c r="AA34" s="7"/>
+      <c r="AB34" s="7"/>
+      <c r="AC34" s="7"/>
+      <c r="AD34" s="7"/>
+      <c r="AE34" s="12">
+        <f t="shared" ref="AE34:AF34" si="21">100/N34</f>
+        <v>5.5248618784530384E-2</v>
+      </c>
+      <c r="AF34" s="12">
+        <f t="shared" si="21"/>
+        <v>5.3619302949061663E-2</v>
+      </c>
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="C35" s="7">
+        <v>153</v>
+      </c>
+      <c r="D35" s="7">
+        <v>46.7</v>
+      </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="G35" s="7"/>
+        <v>603</v>
+      </c>
+      <c r="G35" s="7">
+        <v>16.600000000000001</v>
+      </c>
       <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
+      <c r="I35" s="7">
+        <v>194</v>
+      </c>
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
       <c r="L35" s="7"/>
-      <c r="M35" s="7"/>
+      <c r="M35" s="7">
+        <v>163</v>
+      </c>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
       <c r="S35" t="str">
-        <f>B35</f>
-        <v>AWS US E1</v>
-      </c>
-      <c r="T35" s="11"/>
-      <c r="U35" s="11"/>
+        <f t="shared" si="18"/>
+        <v>Amsterdam</v>
+      </c>
+      <c r="T35" s="12">
+        <f>100/C35</f>
+        <v>0.65359477124183007</v>
+      </c>
+      <c r="U35" s="11">
+        <f t="shared" si="19"/>
+        <v>2.1413276231263381</v>
+      </c>
       <c r="V35" s="11"/>
-      <c r="W35" s="11">
-        <f t="shared" si="10"/>
-        <v>6.2111801242236018</v>
-      </c>
-      <c r="X35" s="11"/>
+      <c r="W35" s="12">
+        <f t="shared" si="20"/>
+        <v>0.16583747927031509</v>
+      </c>
+      <c r="X35" s="11">
+        <f t="shared" ref="X35:X36" si="22">100/G35</f>
+        <v>6.0240963855421681</v>
+      </c>
       <c r="Y35" s="11"/>
-      <c r="Z35" s="11"/>
+      <c r="Z35" s="12">
+        <f t="shared" ref="Z35:AA36" si="23">100/I35</f>
+        <v>0.51546391752577314</v>
+      </c>
       <c r="AA35" s="11"/>
       <c r="AB35" s="11"/>
       <c r="AC35" s="11"/>
-      <c r="AD35" s="11"/>
+      <c r="AD35" s="11">
+        <f t="shared" ref="AD35" si="24">100/M35</f>
+        <v>0.61349693251533743</v>
+      </c>
       <c r="AE35" s="11"/>
       <c r="AF35" s="11"/>
     </row>
     <row r="36" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="C36" s="7">
+        <v>674</v>
+      </c>
+      <c r="D36" s="7">
+        <v>588</v>
+      </c>
       <c r="E36" s="7">
-        <v>21.6</v>
+        <v>83</v>
       </c>
       <c r="F36" s="7">
-        <v>463</v>
+        <v>44.9</v>
       </c>
       <c r="G36" s="7">
-        <v>12.6</v>
+        <v>9.1</v>
       </c>
       <c r="H36" s="7"/>
-      <c r="I36" s="7">
-        <v>5.76</v>
-      </c>
+      <c r="I36" s="7"/>
       <c r="J36" s="7">
-        <v>13.2</v>
-      </c>
-      <c r="K36" s="7">
-        <v>44.3</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="K36" s="7"/>
       <c r="L36" s="7">
-        <v>232</v>
-      </c>
-      <c r="M36" s="7">
-        <v>87.4</v>
-      </c>
-      <c r="N36" s="7">
-        <v>950</v>
-      </c>
-      <c r="O36" s="7">
-        <v>995</v>
-      </c>
+        <v>808</v>
+      </c>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
       <c r="S36" t="str">
-        <f>B36</f>
-        <v>San Diego</v>
-      </c>
-      <c r="T36" s="11"/>
-      <c r="U36" s="11"/>
+        <f t="shared" si="18"/>
+        <v>NewYork</v>
+      </c>
+      <c r="T36" s="12">
+        <f t="shared" ref="T36" si="25">100/C36</f>
+        <v>0.14836795252225518</v>
+      </c>
+      <c r="U36" s="12">
+        <f t="shared" si="19"/>
+        <v>0.17006802721088435</v>
+      </c>
       <c r="V36" s="11">
-        <f t="shared" si="16"/>
-        <v>4.6296296296296298</v>
-      </c>
-      <c r="W36" s="12">
-        <f t="shared" si="10"/>
-        <v>0.21598272138228941</v>
-      </c>
-      <c r="X36" s="11">
-        <f t="shared" ref="X36:X37" si="18">100/G36</f>
-        <v>7.9365079365079367</v>
+        <f t="shared" ref="V36:V38" si="26">100/E36</f>
+        <v>1.2048192771084338</v>
+      </c>
+      <c r="W36" s="11">
+        <f t="shared" si="20"/>
+        <v>2.2271714922048997</v>
+      </c>
+      <c r="X36" s="15">
+        <f t="shared" si="22"/>
+        <v>10.989010989010989</v>
       </c>
       <c r="Y36" s="11"/>
-      <c r="Z36" s="15">
-        <f t="shared" ref="Z36" si="19">100/I36</f>
-        <v>17.361111111111111</v>
-      </c>
-      <c r="AA36" s="11">
-        <f t="shared" ref="AA36:AA37" si="20">100/J36</f>
-        <v>7.5757575757575761</v>
-      </c>
-      <c r="AB36" s="11">
-        <f t="shared" ref="AB36" si="21">100/K36</f>
-        <v>2.2573363431151243</v>
-      </c>
+      <c r="Z36" s="11"/>
+      <c r="AA36" s="12">
+        <f t="shared" si="23"/>
+        <v>0.4329004329004329</v>
+      </c>
+      <c r="AB36" s="11"/>
       <c r="AC36" s="12">
-        <f t="shared" ref="AC36:AF37" si="22">100/L36</f>
-        <v>0.43103448275862066</v>
-      </c>
-      <c r="AD36" s="11">
-        <f t="shared" si="22"/>
-        <v>1.1441647597254003</v>
-      </c>
-      <c r="AE36" s="12">
-        <f t="shared" si="22"/>
-        <v>0.10526315789473684</v>
-      </c>
-      <c r="AF36" s="12">
-        <f t="shared" si="22"/>
-        <v>0.10050251256281408</v>
-      </c>
+        <f t="shared" ref="AC36" si="27">100/L36</f>
+        <v>0.12376237623762376</v>
+      </c>
+      <c r="AD36" s="11"/>
+      <c r="AE36" s="11"/>
+      <c r="AF36" s="11"/>
     </row>
     <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7">
-        <v>514</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
-      <c r="L37" s="7">
-        <v>16.2</v>
-      </c>
+      <c r="L37" s="7"/>
       <c r="M37" s="7"/>
-      <c r="N37" s="7">
-        <v>807</v>
-      </c>
-      <c r="O37" s="7">
-        <v>900</v>
-      </c>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
       <c r="S37" t="str">
-        <f>B37</f>
-        <v>AWS US W2</v>
+        <f t="shared" si="18"/>
+        <v>AWS US E1</v>
       </c>
       <c r="T37" s="11"/>
       <c r="U37" s="11"/>
       <c r="V37" s="11"/>
-      <c r="W37" s="12">
-        <f t="shared" si="10"/>
-        <v>0.19455252918287938</v>
+      <c r="W37" s="11">
+        <f t="shared" si="20"/>
+        <v>6.2111801242236018</v>
       </c>
       <c r="X37" s="11"/>
       <c r="Y37" s="11"/>
       <c r="Z37" s="11"/>
       <c r="AA37" s="11"/>
       <c r="AB37" s="11"/>
-      <c r="AC37" s="11">
-        <f t="shared" si="22"/>
+      <c r="AC37" s="11"/>
+      <c r="AD37" s="11"/>
+      <c r="AE37" s="11"/>
+      <c r="AF37" s="11"/>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7">
+        <v>21.6</v>
+      </c>
+      <c r="F38" s="7">
+        <v>463</v>
+      </c>
+      <c r="G38" s="7">
+        <v>12.6</v>
+      </c>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7">
+        <v>5.76</v>
+      </c>
+      <c r="J38" s="7">
+        <v>13.2</v>
+      </c>
+      <c r="K38" s="7">
+        <v>44.3</v>
+      </c>
+      <c r="L38" s="7">
+        <v>232</v>
+      </c>
+      <c r="M38" s="7">
+        <v>87.4</v>
+      </c>
+      <c r="N38" s="7">
+        <v>950</v>
+      </c>
+      <c r="O38" s="7">
+        <v>995</v>
+      </c>
+      <c r="S38" t="str">
+        <f t="shared" si="18"/>
+        <v>San Diego</v>
+      </c>
+      <c r="T38" s="11"/>
+      <c r="U38" s="11"/>
+      <c r="V38" s="11">
+        <f t="shared" si="26"/>
+        <v>4.6296296296296298</v>
+      </c>
+      <c r="W38" s="12">
+        <f t="shared" si="20"/>
+        <v>0.21598272138228941</v>
+      </c>
+      <c r="X38" s="11">
+        <f t="shared" ref="X38" si="28">100/G38</f>
+        <v>7.9365079365079367</v>
+      </c>
+      <c r="Y38" s="11"/>
+      <c r="Z38" s="15">
+        <f t="shared" ref="Z38" si="29">100/I38</f>
+        <v>17.361111111111111</v>
+      </c>
+      <c r="AA38" s="11">
+        <f t="shared" ref="Z38:AA40" si="30">100/J38</f>
+        <v>7.5757575757575761</v>
+      </c>
+      <c r="AB38" s="11">
+        <f t="shared" ref="AB38" si="31">100/K38</f>
+        <v>2.2573363431151243</v>
+      </c>
+      <c r="AC38" s="12">
+        <f t="shared" ref="AC38:AF40" si="32">100/L38</f>
+        <v>0.43103448275862066</v>
+      </c>
+      <c r="AD38" s="11">
+        <f t="shared" si="32"/>
+        <v>1.1441647597254003</v>
+      </c>
+      <c r="AE38" s="12">
+        <f t="shared" si="32"/>
+        <v>0.10526315789473684</v>
+      </c>
+      <c r="AF38" s="12">
+        <f t="shared" si="32"/>
+        <v>0.10050251256281408</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7">
+        <v>514</v>
+      </c>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7">
+        <v>16.2</v>
+      </c>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7">
+        <v>807</v>
+      </c>
+      <c r="O39" s="7">
+        <v>900</v>
+      </c>
+      <c r="S39" t="str">
+        <f t="shared" si="18"/>
+        <v>AWS US W2</v>
+      </c>
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
+      <c r="V39" s="11"/>
+      <c r="W39" s="12">
+        <f t="shared" si="20"/>
+        <v>0.19455252918287938</v>
+      </c>
+      <c r="X39" s="11"/>
+      <c r="Y39" s="11"/>
+      <c r="Z39" s="11"/>
+      <c r="AA39" s="11"/>
+      <c r="AB39" s="11"/>
+      <c r="AC39" s="11">
+        <f t="shared" si="32"/>
         <v>6.1728395061728394</v>
       </c>
-      <c r="AD37" s="11"/>
-      <c r="AE37" s="12">
-        <f t="shared" si="22"/>
+      <c r="AD39" s="11"/>
+      <c r="AE39" s="12">
+        <f t="shared" si="32"/>
         <v>0.12391573729863693</v>
       </c>
-      <c r="AF37" s="12">
-        <f t="shared" si="22"/>
+      <c r="AF39" s="12">
+        <f t="shared" si="32"/>
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>18</v>
+      </c>
+      <c r="I40" s="7">
+        <v>171</v>
+      </c>
+      <c r="N40" s="7">
+        <v>28.6</v>
+      </c>
+      <c r="S40" t="str">
+        <f t="shared" si="18"/>
+        <v>Korea</v>
+      </c>
+      <c r="Z40" s="12">
+        <f t="shared" ref="Z40" si="33">100/I40</f>
+        <v>0.58479532163742687</v>
+      </c>
+      <c r="AE40" s="11">
+        <f t="shared" si="32"/>
+        <v>3.4965034965034962</v>
+      </c>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Google Japan gftp data
</commit_message>
<xml_diff>
--- a/summary_data/gftp_summary.xlsx
+++ b/summary_data/gftp_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isfiligoi/github/tnrp-net-tests/summary_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C211BA8E-B4FC-9141-9469-F5AB4F4D5734}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A879302A-2C8D-944E-A4B0-106817D247C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18940" xr2:uid="{F871B44F-434F-FB4B-AC1F-99327B90C475}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="32">
   <si>
     <t>Server</t>
   </si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>Azure Korea</t>
+  </si>
+  <si>
+    <t>GCP Australia</t>
+  </si>
+  <si>
+    <t>GCP Japan</t>
   </si>
 </sst>
 </file>
@@ -535,46 +541,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3AE2A42-D91B-564A-AB68-339151ECBD6D}">
-  <dimension ref="A1:AS46"/>
+  <dimension ref="A1:AX46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AP24" sqref="AP24"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AT37" sqref="AT37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="9" max="9" width="13.1640625" customWidth="1"/>
     <col min="15" max="15" width="12.83203125" customWidth="1"/>
-    <col min="32" max="32" width="13.1640625" customWidth="1"/>
+    <col min="33" max="33" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="10" t="str">
+      <c r="AA1" s="10" t="str">
         <f>A1</f>
         <v>GridFTP tests - fast with callback</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="X3" t="s">
+      <c r="AA3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="Y4" t="str">
+      <c r="AB4" t="str">
         <f>B4</f>
         <v>Server</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -630,100 +636,114 @@
         <v>29</v>
       </c>
       <c r="T5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="V5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="W5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="X5" t="str">
+      <c r="X5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA5" t="str">
         <f>A5</f>
         <v>Client</v>
       </c>
-      <c r="Z5" t="str">
+      <c r="AC5" t="str">
         <f>C5</f>
         <v>AWS EU W1</v>
       </c>
-      <c r="AA5" t="str">
+      <c r="AD5" t="str">
         <f>D5</f>
         <v>GCP NL</v>
       </c>
-      <c r="AB5" t="str">
+      <c r="AE5" t="str">
         <f>E5</f>
         <v>Azure EU W</v>
       </c>
-      <c r="AC5" t="str">
+      <c r="AF5" t="str">
         <f>F5</f>
         <v>AWS EU C1</v>
       </c>
-      <c r="AD5" t="str">
+      <c r="AG5" t="str">
         <f>G5</f>
         <v>Amsterdam</v>
       </c>
-      <c r="AE5" t="str">
+      <c r="AH5" t="str">
         <f>H5</f>
         <v>AWS US E1</v>
       </c>
-      <c r="AF5" t="str">
+      <c r="AI5" t="str">
         <f>I5</f>
         <v>Azure US East</v>
       </c>
-      <c r="AG5" t="str">
+      <c r="AJ5" t="str">
         <f>J5</f>
         <v>GCP US E4</v>
       </c>
-      <c r="AH5" t="str">
+      <c r="AK5" t="str">
         <f>K5</f>
         <v>Chicago</v>
       </c>
-      <c r="AI5" t="str">
+      <c r="AL5" t="str">
         <f>L5</f>
         <v>Kansas</v>
       </c>
-      <c r="AJ5" t="str">
+      <c r="AM5" t="str">
         <f>M5</f>
         <v>San Diego</v>
       </c>
-      <c r="AK5" t="str">
+      <c r="AN5" t="str">
         <f>N5</f>
         <v>GCP US W1</v>
       </c>
-      <c r="AL5" t="str">
+      <c r="AO5" t="str">
         <f>O5</f>
         <v>Azure US W2</v>
       </c>
-      <c r="AM5" t="str">
+      <c r="AP5" t="str">
         <f>P5</f>
         <v>AWS US W2</v>
       </c>
-      <c r="AN5" t="str">
+      <c r="AQ5" t="str">
         <f>Q5</f>
         <v>Korea</v>
       </c>
-      <c r="AO5" t="str">
+      <c r="AR5" t="str">
         <f>R5</f>
         <v>AWS Korea</v>
       </c>
-      <c r="AP5" t="str">
+      <c r="AS5" t="str">
         <f>S5</f>
         <v>Azure Korea</v>
       </c>
-      <c r="AQ5" t="str">
-        <f t="shared" ref="AQ5" si="0">T5</f>
+      <c r="AT5" t="str">
+        <f>T5</f>
+        <v>GCP Japan</v>
+      </c>
+      <c r="AU5" t="str">
+        <f>U5</f>
         <v>Australia</v>
       </c>
-      <c r="AR5" t="str">
-        <f t="shared" ref="AR5:AS5" si="1">U5</f>
+      <c r="AV5" t="str">
+        <f>V5</f>
         <v>AWS Australia</v>
       </c>
-      <c r="AS5" t="str">
-        <f t="shared" si="1"/>
+      <c r="AW5" t="str">
+        <f>W5</f>
         <v>Azure Australia</v>
       </c>
-    </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AX5" t="str">
+        <f>X5</f>
+        <v>GCP Australia</v>
+      </c>
+    </row>
+    <row r="6" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -753,49 +773,51 @@
       </c>
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
-      <c r="U6" s="3">
+      <c r="U6" s="3"/>
+      <c r="V6" s="3">
         <v>27.1</v>
       </c>
-      <c r="Y6" t="str">
+      <c r="AB6" t="str">
         <f>B6</f>
         <v>AWS EU C1</v>
       </c>
-      <c r="Z6" s="4">
+      <c r="AC6" s="4">
         <f>100/C6</f>
         <v>5.7471264367816097</v>
       </c>
-      <c r="AA6" s="4"/>
-      <c r="AB6" s="4"/>
-      <c r="AC6" s="14">
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4"/>
+      <c r="AF6" s="14">
         <f>100/F6</f>
         <v>13.333333333333334</v>
       </c>
-      <c r="AD6" s="3"/>
-      <c r="AE6" s="4">
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="4">
         <f>100/H6</f>
         <v>5.1020408163265305</v>
       </c>
-      <c r="AF6" s="4"/>
-      <c r="AG6" s="4"/>
-      <c r="AH6" s="3"/>
-      <c r="AI6" s="3"/>
-      <c r="AJ6" s="3"/>
+      <c r="AI6" s="4"/>
+      <c r="AJ6" s="4"/>
       <c r="AK6" s="3"/>
       <c r="AL6" s="3"/>
       <c r="AM6" s="3"/>
       <c r="AN6" s="3"/>
-      <c r="AO6" s="4">
+      <c r="AO6" s="3"/>
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="3"/>
+      <c r="AR6" s="4">
         <f>100/R6</f>
         <v>3.6496350364963503</v>
       </c>
-      <c r="AP6" s="4"/>
-      <c r="AQ6" s="4"/>
-      <c r="AR6" s="4">
-        <f>100/U6</f>
+      <c r="AS6" s="4"/>
+      <c r="AT6" s="4"/>
+      <c r="AU6" s="4"/>
+      <c r="AV6" s="4">
+        <f>100/V6</f>
         <v>3.6900369003690034</v>
       </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -836,68 +858,70 @@
       </c>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
-      <c r="T7" s="3">
+      <c r="T7" s="3"/>
+      <c r="U7" s="3">
         <v>25</v>
       </c>
-      <c r="U7" s="3"/>
-      <c r="Y7" t="str">
+      <c r="V7" s="3"/>
+      <c r="AB7" t="str">
         <f>B7</f>
         <v>Amsterdam</v>
       </c>
-      <c r="Z7" s="4">
+      <c r="AC7" s="4">
         <f>100/C7</f>
         <v>9.1743119266055047</v>
       </c>
-      <c r="AA7" s="4">
+      <c r="AD7" s="4">
         <f>100/D7</f>
         <v>7.5757575757575761</v>
       </c>
-      <c r="AB7" s="4">
+      <c r="AE7" s="4">
         <f>100/E7</f>
         <v>7.3529411764705888</v>
       </c>
-      <c r="AC7" s="14">
+      <c r="AF7" s="14">
         <f>100/F7</f>
         <v>10.526315789473685</v>
       </c>
-      <c r="AD7" s="3"/>
-      <c r="AE7" s="4">
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="4">
         <f>100/H7</f>
         <v>7.8125</v>
       </c>
-      <c r="AF7" s="4">
+      <c r="AI7" s="4">
         <f>100/I7</f>
         <v>8.064516129032258</v>
       </c>
-      <c r="AG7" s="4">
+      <c r="AJ7" s="4">
         <f>100/J7</f>
         <v>6.9444444444444446</v>
       </c>
-      <c r="AH7" s="4">
+      <c r="AK7" s="4">
         <f>100/K7</f>
         <v>7.8740157480314963</v>
       </c>
-      <c r="AI7" s="3"/>
-      <c r="AJ7" s="4">
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="4">
         <f>100/M7</f>
         <v>7.9365079365079367</v>
       </c>
-      <c r="AK7" s="3"/>
-      <c r="AL7" s="3"/>
-      <c r="AM7" s="3"/>
-      <c r="AN7" s="4">
+      <c r="AN7" s="3"/>
+      <c r="AO7" s="3"/>
+      <c r="AP7" s="3"/>
+      <c r="AQ7" s="4">
         <f>100/Q7</f>
         <v>5.2356020942408374</v>
       </c>
-      <c r="AO7" s="4"/>
-      <c r="AP7" s="4"/>
-      <c r="AQ7" s="4">
-        <f>100/T7</f>
+      <c r="AR7" s="4"/>
+      <c r="AS7" s="4"/>
+      <c r="AT7" s="4"/>
+      <c r="AU7" s="4">
+        <f>100/U7</f>
         <v>4</v>
       </c>
-      <c r="AR7" s="4"/>
-    </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AV7" s="4"/>
+    </row>
+    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>12</v>
       </c>
@@ -948,73 +972,75 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
-      <c r="Y8" t="str">
+      <c r="V8" s="3"/>
+      <c r="AB8" t="str">
         <f>B8</f>
         <v>NewYork</v>
       </c>
-      <c r="Z8" s="4">
+      <c r="AC8" s="4">
         <f>100/C8</f>
         <v>1.0964912280701753</v>
       </c>
-      <c r="AA8" s="4">
+      <c r="AD8" s="4">
         <f>100/D8</f>
         <v>1.1210762331838564</v>
       </c>
-      <c r="AB8" s="4">
+      <c r="AE8" s="4">
         <f>100/E8</f>
         <v>5.7471264367816097</v>
       </c>
-      <c r="AC8" s="4">
+      <c r="AF8" s="4">
         <f>100/F8</f>
         <v>1.1325028312570782</v>
       </c>
-      <c r="AD8" s="4">
+      <c r="AG8" s="4">
         <f>100/G8</f>
         <v>5.5865921787709505</v>
       </c>
-      <c r="AE8" s="14">
+      <c r="AH8" s="14">
         <f>100/H8</f>
         <v>10.526315789473685</v>
       </c>
-      <c r="AF8" s="4">
+      <c r="AI8" s="4">
         <f>100/I8</f>
         <v>6.0240963855421681</v>
       </c>
-      <c r="AG8" s="4">
+      <c r="AJ8" s="4">
         <f>100/J8</f>
         <v>1.1560693641618498</v>
       </c>
-      <c r="AH8" s="14">
+      <c r="AK8" s="14">
         <f>100/K8</f>
         <v>10.989010989010989</v>
       </c>
-      <c r="AI8" s="14">
+      <c r="AL8" s="14">
         <f>100/L8</f>
         <v>11.494252873563219</v>
       </c>
-      <c r="AJ8" s="4"/>
-      <c r="AK8" s="4">
+      <c r="AM8" s="4"/>
+      <c r="AN8" s="4">
         <f>100/N8</f>
         <v>1.1376564277588168</v>
       </c>
-      <c r="AL8" s="4">
+      <c r="AO8" s="4">
         <f>100/O8</f>
         <v>7.6335877862595423</v>
       </c>
-      <c r="AM8" s="4">
+      <c r="AP8" s="4">
         <f>100/P8</f>
         <v>8.4033613445378155</v>
       </c>
-      <c r="AN8" s="4">
+      <c r="AQ8" s="4">
         <f>100/Q8</f>
         <v>6.7567567567567561</v>
       </c>
-      <c r="AO8" s="4"/>
-      <c r="AP8" s="4"/>
-      <c r="AQ8" s="4"/>
       <c r="AR8" s="4"/>
-    </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AS8" s="4"/>
+      <c r="AT8" s="4"/>
+      <c r="AU8" s="4"/>
+      <c r="AV8" s="4"/>
+    </row>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -1044,49 +1070,51 @@
       </c>
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
-      <c r="U9" s="3">
+      <c r="U9" s="3"/>
+      <c r="V9" s="3">
         <v>21.5</v>
       </c>
-      <c r="Y9" t="str">
+      <c r="AB9" t="str">
         <f>B9</f>
         <v>AWS US E1</v>
       </c>
-      <c r="Z9" s="4">
+      <c r="AC9" s="4">
         <f>100/C9</f>
         <v>5.2083333333333339</v>
       </c>
-      <c r="AA9" s="4"/>
-      <c r="AB9" s="4"/>
-      <c r="AC9" s="4">
-        <f t="shared" ref="AC9:AC10" si="2">100/F9</f>
+      <c r="AD9" s="4"/>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4">
+        <f>100/F9</f>
         <v>5.2356020942408374</v>
       </c>
-      <c r="AD9" s="4"/>
-      <c r="AE9" s="14">
+      <c r="AG9" s="4"/>
+      <c r="AH9" s="14">
         <f>100/H9</f>
         <v>14.084507042253522</v>
       </c>
-      <c r="AF9" s="14"/>
-      <c r="AG9" s="14"/>
-      <c r="AH9" s="4"/>
-      <c r="AI9" s="4"/>
-      <c r="AJ9" s="4"/>
+      <c r="AI9" s="14"/>
+      <c r="AJ9" s="14"/>
       <c r="AK9" s="4"/>
       <c r="AL9" s="4"/>
       <c r="AM9" s="4"/>
       <c r="AN9" s="4"/>
-      <c r="AO9" s="4">
-        <f>100/R9</f>
-        <v>4.8780487804878048</v>
-      </c>
+      <c r="AO9" s="4"/>
       <c r="AP9" s="4"/>
       <c r="AQ9" s="4"/>
       <c r="AR9" s="4">
-        <f t="shared" ref="AP9:AS12" si="3">100/U9</f>
+        <f>100/R9</f>
+        <v>4.8780487804878048</v>
+      </c>
+      <c r="AS9" s="4"/>
+      <c r="AT9" s="4"/>
+      <c r="AU9" s="4"/>
+      <c r="AV9" s="4">
+        <f>100/V9</f>
         <v>4.6511627906976747</v>
       </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -1140,97 +1168,111 @@
         <v>15.5</v>
       </c>
       <c r="T10" s="3">
+        <v>14.5</v>
+      </c>
+      <c r="U10" s="3">
         <v>27.7</v>
       </c>
-      <c r="U10" s="3">
+      <c r="V10" s="3">
         <v>43.5</v>
       </c>
-      <c r="V10" s="3">
+      <c r="W10" s="3">
         <v>15.8</v>
       </c>
-      <c r="Y10" t="str">
+      <c r="X10" s="3">
+        <v>13.4</v>
+      </c>
+      <c r="AB10" t="str">
         <f>B10</f>
         <v>San Diego</v>
       </c>
-      <c r="Z10" s="4"/>
-      <c r="AA10" s="4">
+      <c r="AC10" s="4"/>
+      <c r="AD10" s="4">
         <f>100/D10</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="AB10" s="4">
+      <c r="AE10" s="4">
         <f>100/E10</f>
         <v>5.5865921787709505</v>
       </c>
-      <c r="AC10" s="4">
-        <f t="shared" si="2"/>
+      <c r="AF10" s="4">
+        <f>100/F10</f>
         <v>7.6335877862595423</v>
       </c>
-      <c r="AD10" s="4">
+      <c r="AG10" s="4">
         <f>100/G10</f>
         <v>6.25</v>
       </c>
-      <c r="AE10" s="4">
+      <c r="AH10" s="4">
         <f>100/H10</f>
         <v>8.4033613445378155</v>
       </c>
-      <c r="AF10" s="4">
+      <c r="AI10" s="4">
         <f>100/I10</f>
         <v>7.1428571428571432</v>
       </c>
-      <c r="AG10" s="4">
+      <c r="AJ10" s="4">
         <f>100/J10</f>
         <v>7.6923076923076925</v>
       </c>
-      <c r="AH10" s="4">
+      <c r="AK10" s="4">
         <f>100/K10</f>
         <v>8.8495575221238933</v>
       </c>
-      <c r="AI10" s="14">
+      <c r="AL10" s="14">
         <f>100/L10</f>
         <v>12.048192771084336</v>
       </c>
-      <c r="AJ10" s="14">
+      <c r="AM10" s="14">
         <f>100/M10</f>
         <v>12.987012987012987</v>
       </c>
-      <c r="AK10" s="4">
+      <c r="AN10" s="4">
         <f>100/N10</f>
         <v>7.7519379844961236</v>
       </c>
-      <c r="AL10" s="14">
+      <c r="AO10" s="14">
         <f>100/O10</f>
         <v>7.2463768115942022</v>
       </c>
-      <c r="AM10" s="4">
+      <c r="AP10" s="4">
         <f>100/P10</f>
         <v>9.2592592592592595</v>
       </c>
-      <c r="AN10" s="4">
+      <c r="AQ10" s="4">
         <f>100/Q10</f>
         <v>6.9930069930069925</v>
       </c>
-      <c r="AO10" s="4">
+      <c r="AR10" s="4">
         <f>100/R10</f>
         <v>5.3191489361702127</v>
       </c>
-      <c r="AP10" s="4">
-        <f t="shared" si="3"/>
+      <c r="AS10" s="4">
+        <f>100/S10</f>
         <v>6.4516129032258061</v>
       </c>
-      <c r="AQ10" s="4">
+      <c r="AT10" s="4">
         <f>100/T10</f>
+        <v>6.8965517241379306</v>
+      </c>
+      <c r="AU10" s="4">
+        <f>100/U10</f>
         <v>3.6101083032490977</v>
       </c>
-      <c r="AR10" s="4">
-        <f t="shared" si="3"/>
+      <c r="AV10" s="4">
+        <f>100/V10</f>
         <v>2.2988505747126435</v>
       </c>
-      <c r="AS10" s="4">
-        <f t="shared" si="3"/>
+      <c r="AW10" s="4">
+        <f>100/W10</f>
         <v>6.3291139240506329</v>
       </c>
-    </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AX10" s="4">
+        <f>100/X10</f>
+        <v>7.4626865671641793</v>
+      </c>
+    </row>
+    <row r="11" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -1262,52 +1304,54 @@
       </c>
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
-      <c r="U11" s="3">
+      <c r="U11" s="3"/>
+      <c r="V11" s="3">
         <v>21.7</v>
       </c>
-      <c r="Y11" t="str">
+      <c r="AB11" t="str">
         <f>B11</f>
         <v>AWS US W2</v>
       </c>
-      <c r="Z11" s="4">
+      <c r="AC11" s="4">
         <f>100/C11</f>
         <v>4</v>
       </c>
-      <c r="AA11" s="4"/>
-      <c r="AB11" s="4"/>
-      <c r="AC11" s="4">
+      <c r="AD11" s="4"/>
+      <c r="AE11" s="4"/>
+      <c r="AF11" s="4">
         <f>100/F11</f>
         <v>4.9019607843137258</v>
       </c>
-      <c r="AD11" s="4"/>
-      <c r="AE11" s="4">
+      <c r="AG11" s="4"/>
+      <c r="AH11" s="4">
         <f>100/H11</f>
         <v>5.4347826086956523</v>
       </c>
-      <c r="AF11" s="4"/>
-      <c r="AG11" s="4"/>
-      <c r="AH11" s="4"/>
       <c r="AI11" s="4"/>
       <c r="AJ11" s="4"/>
       <c r="AK11" s="4"/>
       <c r="AL11" s="4"/>
-      <c r="AM11" s="14">
+      <c r="AM11" s="4"/>
+      <c r="AN11" s="4"/>
+      <c r="AO11" s="4"/>
+      <c r="AP11" s="14">
         <f>100/P11</f>
         <v>12.658227848101266</v>
       </c>
-      <c r="AN11" s="4"/>
-      <c r="AO11" s="4">
+      <c r="AQ11" s="4"/>
+      <c r="AR11" s="4">
         <f>100/R11</f>
         <v>5</v>
       </c>
-      <c r="AP11" s="4"/>
-      <c r="AQ11" s="4"/>
-      <c r="AR11" s="4">
-        <f t="shared" si="3"/>
+      <c r="AS11" s="4"/>
+      <c r="AT11" s="4"/>
+      <c r="AU11" s="4"/>
+      <c r="AV11" s="4">
+        <f>100/V11</f>
         <v>4.6082949308755765</v>
       </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>17</v>
       </c>
@@ -1338,13 +1382,11 @@
       </c>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
-      <c r="Y12" t="str">
+      <c r="V12" s="3"/>
+      <c r="AB12" t="str">
         <f>B12</f>
         <v>Korea</v>
       </c>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="4"/>
-      <c r="AB12" s="4"/>
       <c r="AC12" s="4"/>
       <c r="AD12" s="4"/>
       <c r="AE12" s="4"/>
@@ -1352,55 +1394,59 @@
       <c r="AG12" s="4"/>
       <c r="AH12" s="4"/>
       <c r="AI12" s="4"/>
-      <c r="AJ12" s="4">
-        <f>100/M12</f>
-        <v>4.8543689320388346</v>
-      </c>
+      <c r="AJ12" s="4"/>
       <c r="AK12" s="4"/>
       <c r="AL12" s="4"/>
       <c r="AM12" s="4">
+        <f>100/M12</f>
+        <v>4.8543689320388346</v>
+      </c>
+      <c r="AN12" s="4"/>
+      <c r="AO12" s="4"/>
+      <c r="AP12" s="4">
         <f>100/P12</f>
         <v>0.77519379844961245</v>
       </c>
-      <c r="AN12" s="4"/>
-      <c r="AO12" s="14">
+      <c r="AQ12" s="4"/>
+      <c r="AR12" s="14">
         <f>100/R12</f>
         <v>10.309278350515465</v>
       </c>
-      <c r="AP12" s="4">
-        <f t="shared" si="3"/>
+      <c r="AS12" s="4">
+        <f>100/S12</f>
         <v>4.7393364928909953</v>
       </c>
-      <c r="AQ12" s="14"/>
-      <c r="AR12" s="4"/>
-    </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT12" s="4"/>
+      <c r="AU12" s="14"/>
+      <c r="AV12" s="4"/>
+    </row>
+    <row r="15" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="X15" s="9" t="str">
+      <c r="AA15" s="9" t="str">
         <f>A15</f>
         <v>GridFTP tests - single threaded, multiple processes</v>
       </c>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="X17" t="s">
+      <c r="AA17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>0</v>
       </c>
-      <c r="Y18" t="str">
+      <c r="AB18" t="str">
         <f>B18</f>
         <v>Server</v>
       </c>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -1456,100 +1502,114 @@
         <v>29</v>
       </c>
       <c r="T19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="U19" t="s">
+      <c r="V19" t="s">
         <v>11</v>
       </c>
-      <c r="V19" s="1" t="s">
+      <c r="W19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="X19" t="str">
+      <c r="X19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA19" t="str">
         <f>A19</f>
         <v>Client</v>
       </c>
-      <c r="Z19" t="str">
+      <c r="AC19" t="str">
         <f>C19</f>
         <v>AWS EU W1</v>
       </c>
-      <c r="AA19" t="str">
+      <c r="AD19" t="str">
         <f>D19</f>
         <v>GCP NL</v>
       </c>
-      <c r="AB19" t="str">
-        <f t="shared" ref="AB19" si="4">E19</f>
+      <c r="AE19" t="str">
+        <f>E19</f>
         <v>Azure EU W</v>
       </c>
-      <c r="AC19" t="str">
+      <c r="AF19" t="str">
         <f>F19</f>
         <v>AWS EU C1</v>
       </c>
-      <c r="AD19" t="str">
+      <c r="AG19" t="str">
         <f>G19</f>
         <v>Amsterdam</v>
       </c>
-      <c r="AE19" t="str">
+      <c r="AH19" t="str">
         <f>H19</f>
         <v>AWS US E1</v>
       </c>
-      <c r="AF19" t="str">
-        <f t="shared" ref="AF19" si="5">I19</f>
+      <c r="AI19" t="str">
+        <f>I19</f>
         <v>Azure US East</v>
       </c>
-      <c r="AG19" t="str">
-        <f t="shared" ref="AG19" si="6">J19</f>
+      <c r="AJ19" t="str">
+        <f>J19</f>
         <v>GCP US E4</v>
       </c>
-      <c r="AH19" t="str">
+      <c r="AK19" t="str">
         <f>K19</f>
         <v>Chicago</v>
       </c>
-      <c r="AI19" t="str">
+      <c r="AL19" t="str">
         <f>L19</f>
         <v>Kansas</v>
       </c>
-      <c r="AJ19" t="str">
+      <c r="AM19" t="str">
         <f>M19</f>
         <v>San Diego</v>
       </c>
-      <c r="AK19" t="str">
+      <c r="AN19" t="str">
         <f>N19</f>
         <v>GCP US W1</v>
       </c>
-      <c r="AL19" t="str">
+      <c r="AO19" t="str">
         <f>O19</f>
         <v>Azure US W2</v>
       </c>
-      <c r="AM19" t="str">
+      <c r="AP19" t="str">
         <f>P19</f>
         <v>AWS US W2</v>
       </c>
-      <c r="AN19" t="str">
+      <c r="AQ19" t="str">
         <f>Q19</f>
         <v>Korea</v>
       </c>
-      <c r="AO19" t="str">
+      <c r="AR19" t="str">
         <f>R19</f>
         <v>AWS Korea</v>
       </c>
-      <c r="AP19" t="str">
+      <c r="AS19" t="str">
         <f>S19</f>
         <v>Azure Korea</v>
       </c>
-      <c r="AQ19" t="str">
-        <f t="shared" ref="AQ19" si="7">T19</f>
+      <c r="AT19" t="str">
+        <f>T19</f>
+        <v>GCP Japan</v>
+      </c>
+      <c r="AU19" t="str">
+        <f>U19</f>
         <v>Australia</v>
       </c>
-      <c r="AR19" t="str">
-        <f t="shared" ref="AR19:AS19" si="8">U19</f>
+      <c r="AV19" t="str">
+        <f>V19</f>
         <v>AWS Australia</v>
       </c>
-      <c r="AS19" t="str">
-        <f t="shared" si="8"/>
+      <c r="AW19" t="str">
+        <f>W19</f>
         <v>Azure Australia</v>
       </c>
-    </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AX19" t="str">
+        <f>X19</f>
+        <v>GCP Australia</v>
+      </c>
+    </row>
+    <row r="20" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>2</v>
       </c>
@@ -1579,49 +1639,51 @@
       </c>
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
-      <c r="U20" s="5">
+      <c r="U20" s="5"/>
+      <c r="V20" s="5">
         <v>122</v>
       </c>
-      <c r="Y20" t="str">
+      <c r="AB20" t="str">
         <f>B20</f>
         <v>AWS EU C1</v>
       </c>
-      <c r="Z20" s="6">
+      <c r="AC20" s="6">
         <f>100/C20</f>
         <v>1.893939393939394</v>
       </c>
-      <c r="AA20" s="6"/>
-      <c r="AB20" s="6"/>
-      <c r="AC20" s="13">
+      <c r="AD20" s="6"/>
+      <c r="AE20" s="6"/>
+      <c r="AF20" s="13">
         <f>100/F20</f>
         <v>30.3951367781155</v>
       </c>
-      <c r="AD20" s="5"/>
-      <c r="AE20" s="6">
+      <c r="AG20" s="5"/>
+      <c r="AH20" s="6">
         <f>100/H20</f>
         <v>1.8975332068311195</v>
       </c>
-      <c r="AF20" s="6"/>
-      <c r="AG20" s="6"/>
-      <c r="AH20" s="5"/>
-      <c r="AI20" s="5"/>
-      <c r="AJ20" s="5"/>
+      <c r="AI20" s="6"/>
+      <c r="AJ20" s="6"/>
       <c r="AK20" s="5"/>
       <c r="AL20" s="5"/>
       <c r="AM20" s="5"/>
       <c r="AN20" s="5"/>
-      <c r="AO20" s="6">
+      <c r="AO20" s="5"/>
+      <c r="AP20" s="5"/>
+      <c r="AQ20" s="5"/>
+      <c r="AR20" s="6">
         <f>100/R20</f>
         <v>1.0504201680672269</v>
       </c>
-      <c r="AP20" s="6"/>
-      <c r="AQ20" s="6"/>
-      <c r="AR20" s="6">
-        <f t="shared" ref="AR20" si="9">100/U20</f>
+      <c r="AS20" s="6"/>
+      <c r="AT20" s="6"/>
+      <c r="AU20" s="6"/>
+      <c r="AV20" s="6">
+        <f>100/V20</f>
         <v>0.81967213114754101</v>
       </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>3</v>
       </c>
@@ -1662,68 +1724,70 @@
       </c>
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
-      <c r="T21" s="5">
+      <c r="T21" s="5"/>
+      <c r="U21" s="5">
         <v>21.4</v>
       </c>
-      <c r="U21" s="5"/>
-      <c r="Y21" t="str">
+      <c r="V21" s="5"/>
+      <c r="AB21" t="str">
         <f>B21</f>
         <v>Amsterdam</v>
       </c>
-      <c r="Z21" s="6">
+      <c r="AC21" s="6">
         <f>100/C21</f>
         <v>9.3457943925233646</v>
       </c>
-      <c r="AA21" s="13">
+      <c r="AD21" s="13">
         <f>100/D21</f>
         <v>10.75268817204301</v>
       </c>
-      <c r="AB21" s="13">
+      <c r="AE21" s="13">
         <f>100/E21</f>
         <v>9.7087378640776691</v>
       </c>
-      <c r="AC21" s="6">
+      <c r="AF21" s="6">
         <f>100/F21</f>
         <v>9.5238095238095237</v>
       </c>
-      <c r="AD21" s="6"/>
-      <c r="AE21" s="6">
+      <c r="AG21" s="6"/>
+      <c r="AH21" s="6">
         <f>100/H21</f>
         <v>3.1446540880503142</v>
       </c>
-      <c r="AF21" s="6">
+      <c r="AI21" s="6">
         <f>100/I21</f>
         <v>6.8027210884353746</v>
       </c>
-      <c r="AG21" s="6">
+      <c r="AJ21" s="6">
         <f>100/J21</f>
         <v>5.7142857142857144</v>
       </c>
-      <c r="AH21" s="6">
-        <f t="shared" ref="AH21:AH24" si="10">100/K21</f>
+      <c r="AK21" s="6">
+        <f>100/K21</f>
         <v>7.1942446043165464</v>
       </c>
-      <c r="AI21" s="6"/>
-      <c r="AJ21" s="6">
+      <c r="AL21" s="6"/>
+      <c r="AM21" s="6">
         <f>100/M21</f>
         <v>8</v>
       </c>
-      <c r="AK21" s="6"/>
-      <c r="AL21" s="6"/>
-      <c r="AM21" s="6"/>
-      <c r="AN21" s="6">
-        <f>100/Q21</f>
-        <v>4.2553191489361701</v>
-      </c>
+      <c r="AN21" s="6"/>
       <c r="AO21" s="6"/>
       <c r="AP21" s="6"/>
       <c r="AQ21" s="6">
-        <f>100/T21</f>
+        <f>100/Q21</f>
+        <v>4.2553191489361701</v>
+      </c>
+      <c r="AR21" s="6"/>
+      <c r="AS21" s="6"/>
+      <c r="AT21" s="6"/>
+      <c r="AU21" s="6">
+        <f>100/U21</f>
         <v>4.6728971962616823</v>
       </c>
-      <c r="AR21" s="6"/>
-    </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AV21" s="6"/>
+    </row>
+    <row r="22" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>12</v>
       </c>
@@ -1770,67 +1834,69 @@
       <c r="S22" s="5"/>
       <c r="T22" s="5"/>
       <c r="U22" s="5"/>
-      <c r="Y22" t="str">
+      <c r="V22" s="5"/>
+      <c r="AB22" t="str">
         <f>B22</f>
         <v>NewYork</v>
       </c>
-      <c r="Z22" s="6">
+      <c r="AC22" s="6">
         <f>100/C22</f>
         <v>1.0834236186348862</v>
       </c>
-      <c r="AA22" s="6">
+      <c r="AD22" s="6">
         <f>100/D22</f>
         <v>1.1210762331838564</v>
       </c>
-      <c r="AB22" s="6">
+      <c r="AE22" s="6">
         <f>100/E22</f>
         <v>2.6737967914438503</v>
       </c>
-      <c r="AC22" s="6">
+      <c r="AF22" s="6">
         <f>100/F22</f>
         <v>1.0893246187363834</v>
       </c>
-      <c r="AD22" s="6">
+      <c r="AG22" s="6">
         <f>100/G22</f>
         <v>3.4482758620689653</v>
       </c>
-      <c r="AE22" s="13">
+      <c r="AH22" s="13">
         <f>100/H22</f>
         <v>10.309278350515465</v>
       </c>
-      <c r="AF22" s="6">
+      <c r="AI22" s="6">
         <f>100/I22</f>
         <v>3.5714285714285716</v>
       </c>
-      <c r="AG22" s="6">
+      <c r="AJ22" s="6">
         <f>100/J22</f>
         <v>1.1534025374855825</v>
       </c>
-      <c r="AH22" s="13">
-        <f t="shared" si="10"/>
+      <c r="AK22" s="13">
+        <f>100/K22</f>
         <v>13.698630136986301</v>
       </c>
-      <c r="AI22" s="6"/>
-      <c r="AJ22" s="6"/>
-      <c r="AK22" s="6">
+      <c r="AL22" s="6"/>
+      <c r="AM22" s="6"/>
+      <c r="AN22" s="6">
         <f>100/N22</f>
         <v>1.0718113612004287</v>
       </c>
-      <c r="AL22" s="6">
+      <c r="AO22" s="6">
         <f>100/O22</f>
         <v>7.3529411764705888</v>
       </c>
-      <c r="AM22" s="6">
+      <c r="AP22" s="6">
         <f>100/P22</f>
         <v>2.7700831024930745</v>
       </c>
-      <c r="AN22" s="6"/>
-      <c r="AO22" s="6"/>
-      <c r="AP22" s="6"/>
       <c r="AQ22" s="6"/>
       <c r="AR22" s="6"/>
-    </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AS22" s="6"/>
+      <c r="AT22" s="6"/>
+      <c r="AU22" s="6"/>
+      <c r="AV22" s="6"/>
+    </row>
+    <row r="23" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>8</v>
       </c>
@@ -1855,24 +1921,22 @@
       <c r="S23" s="5"/>
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
-      <c r="Y23" t="str">
+      <c r="V23" s="5"/>
+      <c r="AB23" t="str">
         <f>B23</f>
         <v>AWS US E1</v>
       </c>
-      <c r="Z23" s="6"/>
-      <c r="AA23" s="6"/>
-      <c r="AB23" s="6"/>
       <c r="AC23" s="6"/>
       <c r="AD23" s="6"/>
-      <c r="AE23" s="13">
+      <c r="AE23" s="6"/>
+      <c r="AF23" s="6"/>
+      <c r="AG23" s="6"/>
+      <c r="AH23" s="13">
         <f>100/H23</f>
         <v>30.120481927710845</v>
       </c>
-      <c r="AF23" s="13"/>
-      <c r="AG23" s="13"/>
-      <c r="AH23" s="6"/>
-      <c r="AI23" s="6"/>
-      <c r="AJ23" s="6"/>
+      <c r="AI23" s="13"/>
+      <c r="AJ23" s="13"/>
       <c r="AK23" s="6"/>
       <c r="AL23" s="6"/>
       <c r="AM23" s="6"/>
@@ -1881,8 +1945,12 @@
       <c r="AP23" s="6"/>
       <c r="AQ23" s="6"/>
       <c r="AR23" s="6"/>
-    </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AS23" s="6"/>
+      <c r="AT23" s="6"/>
+      <c r="AU23" s="6"/>
+      <c r="AV23" s="6"/>
+    </row>
+    <row r="24" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>6</v>
       </c>
@@ -1934,94 +2002,108 @@
         <v>24.5</v>
       </c>
       <c r="T24" s="5">
+        <v>18.8</v>
+      </c>
+      <c r="U24" s="5">
         <v>28.8</v>
       </c>
-      <c r="U24" s="5">
+      <c r="V24" s="5">
         <v>74.5</v>
       </c>
-      <c r="V24" s="5">
+      <c r="W24" s="5">
         <v>27.6</v>
       </c>
-      <c r="Y24" t="str">
+      <c r="X24" s="5">
+        <v>25.2</v>
+      </c>
+      <c r="AB24" t="str">
         <f>B24</f>
         <v>San Diego</v>
       </c>
-      <c r="Z24" s="6"/>
-      <c r="AA24" s="6">
+      <c r="AC24" s="6"/>
+      <c r="AD24" s="6">
         <f>100/D24</f>
         <v>3.9525691699604741</v>
       </c>
-      <c r="AB24" s="6">
+      <c r="AE24" s="6">
         <f>100/E24</f>
         <v>3.90625</v>
       </c>
-      <c r="AC24" s="6">
+      <c r="AF24" s="6">
         <f>100/F24</f>
         <v>1.8248175182481752</v>
       </c>
-      <c r="AD24" s="6">
+      <c r="AG24" s="6">
         <f>100/G24</f>
         <v>4.6296296296296298</v>
       </c>
-      <c r="AE24" s="6">
+      <c r="AH24" s="6">
         <f>100/H24</f>
         <v>3.9215686274509802</v>
       </c>
-      <c r="AF24" s="6">
+      <c r="AI24" s="6">
         <f>100/I24</f>
         <v>8.5470085470085468</v>
       </c>
-      <c r="AG24" s="6">
+      <c r="AJ24" s="6">
         <f>100/J24</f>
         <v>8.4033613445378155</v>
       </c>
-      <c r="AH24" s="6">
-        <f t="shared" si="10"/>
+      <c r="AK24" s="6">
+        <f>100/K24</f>
         <v>8.7719298245614024</v>
       </c>
-      <c r="AI24" s="6"/>
-      <c r="AJ24" s="13">
-        <f t="shared" ref="AJ24" si="11">100/M24</f>
+      <c r="AL24" s="6"/>
+      <c r="AM24" s="13">
+        <f>100/M24</f>
         <v>43.478260869565219</v>
       </c>
-      <c r="AK24" s="6">
+      <c r="AN24" s="6">
         <f>100/N24</f>
         <v>8.9285714285714288</v>
       </c>
-      <c r="AL24" s="6">
-        <f t="shared" ref="AL24" si="12">100/O24</f>
+      <c r="AO24" s="6">
+        <f>100/O24</f>
         <v>4.5454545454545459</v>
       </c>
-      <c r="AM24" s="6">
+      <c r="AP24" s="6">
         <f>100/P24</f>
         <v>7.8125</v>
       </c>
-      <c r="AN24" s="6">
+      <c r="AQ24" s="6">
         <f>100/Q24</f>
         <v>1.9685039370078741</v>
       </c>
-      <c r="AO24" s="6">
+      <c r="AR24" s="6">
         <f>100/R24</f>
         <v>1.6260162601626016</v>
       </c>
-      <c r="AP24" s="6">
-        <f t="shared" ref="AP24:AS26" si="13">100/S24</f>
+      <c r="AS24" s="6">
+        <f>100/S24</f>
         <v>4.0816326530612246</v>
       </c>
-      <c r="AQ24" s="6">
+      <c r="AT24" s="6">
         <f>100/T24</f>
+        <v>5.3191489361702127</v>
+      </c>
+      <c r="AU24" s="6">
+        <f>100/U24</f>
         <v>3.4722222222222223</v>
       </c>
-      <c r="AR24" s="6">
-        <f t="shared" si="13"/>
+      <c r="AV24" s="6">
+        <f>100/V24</f>
         <v>1.3422818791946309</v>
       </c>
-      <c r="AS24" s="6">
-        <f t="shared" si="13"/>
+      <c r="AW24" s="6">
+        <f>100/W24</f>
         <v>3.6231884057971011</v>
       </c>
-    </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AX24" s="6">
+        <f>100/X24</f>
+        <v>3.9682539682539684</v>
+      </c>
+    </row>
+    <row r="25" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>7</v>
       </c>
@@ -2053,52 +2135,54 @@
       </c>
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
-      <c r="U25" s="5">
+      <c r="U25" s="5"/>
+      <c r="V25" s="5">
         <v>62.5</v>
       </c>
-      <c r="Y25" t="str">
+      <c r="AB25" t="str">
         <f>B25</f>
         <v>AWS US W2</v>
       </c>
-      <c r="Z25" s="6">
+      <c r="AC25" s="6">
         <f>100/C25</f>
         <v>1.1560693641618498</v>
       </c>
-      <c r="AA25" s="6"/>
-      <c r="AB25" s="6"/>
-      <c r="AC25" s="6">
+      <c r="AD25" s="6"/>
+      <c r="AE25" s="6"/>
+      <c r="AF25" s="6">
         <f>100/F25</f>
         <v>0.72992700729927007</v>
       </c>
-      <c r="AD25" s="6"/>
-      <c r="AE25" s="6">
+      <c r="AG25" s="6"/>
+      <c r="AH25" s="6">
         <f>100/H25</f>
         <v>1.8382352941176472</v>
       </c>
-      <c r="AF25" s="6"/>
-      <c r="AG25" s="6"/>
-      <c r="AH25" s="6"/>
       <c r="AI25" s="6"/>
       <c r="AJ25" s="6"/>
       <c r="AK25" s="6"/>
       <c r="AL25" s="6"/>
-      <c r="AM25" s="13">
+      <c r="AM25" s="6"/>
+      <c r="AN25" s="6"/>
+      <c r="AO25" s="6"/>
+      <c r="AP25" s="13">
         <f>100/P25</f>
         <v>30.303030303030305</v>
       </c>
-      <c r="AN25" s="6"/>
-      <c r="AO25" s="6">
+      <c r="AQ25" s="6"/>
+      <c r="AR25" s="6">
         <f>100/R25</f>
         <v>1.8050541516245489</v>
       </c>
-      <c r="AP25" s="6"/>
-      <c r="AQ25" s="6"/>
-      <c r="AR25" s="6">
-        <f t="shared" si="13"/>
+      <c r="AS25" s="6"/>
+      <c r="AT25" s="6"/>
+      <c r="AU25" s="6"/>
+      <c r="AV25" s="6">
+        <f>100/V25</f>
         <v>1.6</v>
       </c>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>17</v>
       </c>
@@ -2129,13 +2213,11 @@
       </c>
       <c r="T26" s="5"/>
       <c r="U26" s="5"/>
-      <c r="Y26" t="str">
+      <c r="V26" s="5"/>
+      <c r="AB26" t="str">
         <f>B26</f>
         <v>Korea</v>
       </c>
-      <c r="Z26" s="6"/>
-      <c r="AA26" s="6"/>
-      <c r="AB26" s="6"/>
       <c r="AC26" s="6"/>
       <c r="AD26" s="6"/>
       <c r="AE26" s="6"/>
@@ -2143,32 +2225,33 @@
       <c r="AG26" s="6"/>
       <c r="AH26" s="6"/>
       <c r="AI26" s="6"/>
-      <c r="AJ26" s="6">
-        <f>100/M26</f>
-        <v>5.4644808743169397</v>
-      </c>
+      <c r="AJ26" s="6"/>
       <c r="AK26" s="6"/>
       <c r="AL26" s="6"/>
       <c r="AM26" s="6">
+        <f>100/M26</f>
+        <v>5.4644808743169397</v>
+      </c>
+      <c r="AN26" s="6"/>
+      <c r="AO26" s="6"/>
+      <c r="AP26" s="6">
         <f>100/P26</f>
         <v>0.5714285714285714</v>
       </c>
-      <c r="AN26" s="6"/>
-      <c r="AO26" s="6">
+      <c r="AQ26" s="6"/>
+      <c r="AR26" s="6">
         <f>100/R26</f>
         <v>7.7519379844961236</v>
       </c>
-      <c r="AP26" s="6">
-        <f t="shared" si="13"/>
+      <c r="AS26" s="6">
+        <f>100/S26</f>
         <v>2.0618556701030926</v>
       </c>
-      <c r="AQ26" s="6"/>
-      <c r="AR26" s="6"/>
-    </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="Z27" s="2"/>
-      <c r="AA27" s="2"/>
-      <c r="AB27" s="2"/>
+      <c r="AT26" s="6"/>
+      <c r="AU26" s="6"/>
+      <c r="AV26" s="6"/>
+    </row>
+    <row r="27" spans="1:50" x14ac:dyDescent="0.2">
       <c r="AC27" s="2"/>
       <c r="AD27" s="2"/>
       <c r="AE27" s="2"/>
@@ -2185,34 +2268,38 @@
       <c r="AP27" s="2"/>
       <c r="AQ27" s="2"/>
       <c r="AR27" s="2"/>
-    </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AS27" s="2"/>
+      <c r="AT27" s="2"/>
+      <c r="AU27" s="2"/>
+      <c r="AV27" s="2"/>
+    </row>
+    <row r="29" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="X29" s="8" t="str">
+      <c r="AA29" s="8" t="str">
         <f>A29</f>
         <v>GridFTP tests - single threaded, single process</v>
       </c>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>13</v>
       </c>
-      <c r="X31" t="s">
+      <c r="AA31" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>0</v>
       </c>
-      <c r="Y32" t="str">
+      <c r="AB32" t="str">
         <f>B32</f>
         <v>Server</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -2268,100 +2355,114 @@
         <v>29</v>
       </c>
       <c r="T33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U33" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="U33" t="s">
+      <c r="V33" t="s">
         <v>11</v>
       </c>
-      <c r="V33" s="1" t="s">
+      <c r="W33" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="X33" t="str">
+      <c r="X33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA33" t="str">
         <f>A33</f>
         <v>Client</v>
       </c>
-      <c r="Z33" t="str">
+      <c r="AC33" t="str">
         <f>C33</f>
         <v>AWS EU W1</v>
       </c>
-      <c r="AA33" t="str">
+      <c r="AD33" t="str">
         <f>D33</f>
         <v>GCP NL</v>
       </c>
-      <c r="AB33" t="str">
-        <f t="shared" ref="AB33" si="14">E33</f>
+      <c r="AE33" t="str">
+        <f>E33</f>
         <v>Azure EU W</v>
       </c>
-      <c r="AC33" t="str">
+      <c r="AF33" t="str">
         <f>F33</f>
         <v>AWS EU C1</v>
       </c>
-      <c r="AD33" t="str">
+      <c r="AG33" t="str">
         <f>G33</f>
         <v>Amsterdam</v>
       </c>
-      <c r="AE33" t="str">
+      <c r="AH33" t="str">
         <f>H33</f>
         <v>AWS US E1</v>
       </c>
-      <c r="AF33" t="str">
-        <f t="shared" ref="AF33" si="15">I33</f>
+      <c r="AI33" t="str">
+        <f>I33</f>
         <v>Azure US East</v>
       </c>
-      <c r="AG33" t="str">
-        <f t="shared" ref="AG33" si="16">J33</f>
+      <c r="AJ33" t="str">
+        <f>J33</f>
         <v>GCP US E4</v>
       </c>
-      <c r="AH33" t="str">
+      <c r="AK33" t="str">
         <f>K33</f>
         <v>Chicago</v>
       </c>
-      <c r="AI33" t="str">
+      <c r="AL33" t="str">
         <f>L33</f>
         <v>Kansas</v>
       </c>
-      <c r="AJ33" t="str">
+      <c r="AM33" t="str">
         <f>M33</f>
         <v>San Diego</v>
       </c>
-      <c r="AK33" t="str">
+      <c r="AN33" t="str">
         <f>N33</f>
         <v>GCP US W1</v>
       </c>
-      <c r="AL33" t="str">
+      <c r="AO33" t="str">
         <f>O33</f>
         <v>Azure US W2</v>
       </c>
-      <c r="AM33" t="str">
+      <c r="AP33" t="str">
         <f>P33</f>
         <v>AWS US W2</v>
       </c>
-      <c r="AN33" t="str">
+      <c r="AQ33" t="str">
         <f>Q33</f>
         <v>Korea</v>
       </c>
-      <c r="AO33" t="str">
+      <c r="AR33" t="str">
         <f>R33</f>
         <v>AWS Korea</v>
       </c>
-      <c r="AP33" t="str">
+      <c r="AS33" t="str">
         <f>S33</f>
         <v>Azure Korea</v>
       </c>
-      <c r="AQ33" t="str">
-        <f t="shared" ref="AQ33" si="17">T33</f>
+      <c r="AT33" t="str">
+        <f>T33</f>
+        <v>GCP Japan</v>
+      </c>
+      <c r="AU33" t="str">
+        <f>U33</f>
         <v>Australia</v>
       </c>
-      <c r="AR33" t="str">
-        <f t="shared" ref="AR33:AS33" si="18">U33</f>
+      <c r="AV33" t="str">
+        <f>V33</f>
         <v>AWS Australia</v>
       </c>
-      <c r="AS33" t="str">
-        <f t="shared" si="18"/>
+      <c r="AW33" t="str">
+        <f>W33</f>
         <v>Azure Australia</v>
       </c>
-    </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AX33" t="str">
+        <f>X33</f>
+        <v>GCP Australia</v>
+      </c>
+    </row>
+    <row r="34" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>2</v>
       </c>
@@ -2391,49 +2492,51 @@
       </c>
       <c r="S34" s="7"/>
       <c r="T34" s="7"/>
-      <c r="U34" s="7">
+      <c r="U34" s="7"/>
+      <c r="V34" s="7">
         <v>1865</v>
       </c>
-      <c r="Y34" t="str">
+      <c r="AB34" t="str">
         <f>B34</f>
         <v>AWS EU C1</v>
       </c>
-      <c r="Z34" s="12">
+      <c r="AC34" s="12">
         <f>100/C34</f>
         <v>0.59880239520958078</v>
       </c>
-      <c r="AA34" s="12"/>
-      <c r="AB34" s="12"/>
-      <c r="AC34" s="15">
+      <c r="AD34" s="12"/>
+      <c r="AE34" s="12"/>
+      <c r="AF34" s="15">
         <f>100/F34</f>
         <v>11.627906976744187</v>
       </c>
-      <c r="AD34" s="7"/>
-      <c r="AE34" s="12">
+      <c r="AG34" s="7"/>
+      <c r="AH34" s="12">
         <f>100/H34</f>
         <v>0.17667844522968199</v>
       </c>
-      <c r="AF34" s="12"/>
-      <c r="AG34" s="12"/>
-      <c r="AH34" s="7"/>
-      <c r="AI34" s="7"/>
-      <c r="AJ34" s="7"/>
+      <c r="AI34" s="12"/>
+      <c r="AJ34" s="12"/>
       <c r="AK34" s="7"/>
       <c r="AL34" s="7"/>
       <c r="AM34" s="7"/>
       <c r="AN34" s="7"/>
-      <c r="AO34" s="12">
+      <c r="AO34" s="7"/>
+      <c r="AP34" s="7"/>
+      <c r="AQ34" s="7"/>
+      <c r="AR34" s="12">
         <f>100/R34</f>
         <v>5.5248618784530384E-2</v>
       </c>
-      <c r="AP34" s="12"/>
-      <c r="AQ34" s="12"/>
-      <c r="AR34" s="12">
-        <f t="shared" ref="AR34" si="19">100/U34</f>
+      <c r="AS34" s="12"/>
+      <c r="AT34" s="12"/>
+      <c r="AU34" s="12"/>
+      <c r="AV34" s="12">
+        <f>100/V34</f>
         <v>5.3619302949061663E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>3</v>
       </c>
@@ -2474,65 +2577,67 @@
       </c>
       <c r="R35" s="7"/>
       <c r="S35" s="7"/>
-      <c r="T35" s="7">
+      <c r="T35" s="7"/>
+      <c r="U35" s="7">
         <v>53.2</v>
       </c>
-      <c r="U35" s="7"/>
-      <c r="Y35" t="str">
+      <c r="V35" s="7"/>
+      <c r="AB35" t="str">
         <f>B35</f>
         <v>Amsterdam</v>
       </c>
-      <c r="Z35" s="12">
+      <c r="AC35" s="12">
         <f>100/C35</f>
         <v>0.65359477124183007</v>
       </c>
-      <c r="AA35" s="11">
+      <c r="AD35" s="11">
         <f>100/D35</f>
         <v>6.2893081761006284</v>
       </c>
-      <c r="AB35" s="11">
+      <c r="AE35" s="11">
         <f>100/E35</f>
         <v>3.3444816053511706</v>
       </c>
-      <c r="AC35" s="11">
+      <c r="AF35" s="11">
         <f>100/F35</f>
         <v>2.1413276231263381</v>
       </c>
-      <c r="AD35" s="11"/>
-      <c r="AE35" s="12">
+      <c r="AG35" s="11"/>
+      <c r="AH35" s="12">
         <f>100/H35</f>
         <v>0.16583747927031509</v>
       </c>
-      <c r="AF35" s="12">
+      <c r="AI35" s="12">
         <f>100/I35</f>
         <v>0.36231884057971014</v>
       </c>
-      <c r="AG35" s="12"/>
-      <c r="AH35" s="11">
-        <f t="shared" ref="AH35:AH36" si="20">100/K35</f>
+      <c r="AJ35" s="12"/>
+      <c r="AK35" s="11">
+        <f>100/K35</f>
         <v>6.0240963855421681</v>
       </c>
-      <c r="AI35" s="11"/>
-      <c r="AJ35" s="12">
+      <c r="AL35" s="11"/>
+      <c r="AM35" s="12">
         <f>100/M35</f>
         <v>0.51546391752577314</v>
       </c>
-      <c r="AK35" s="11"/>
-      <c r="AL35" s="11"/>
-      <c r="AM35" s="11"/>
-      <c r="AN35" s="12">
+      <c r="AN35" s="11"/>
+      <c r="AO35" s="11"/>
+      <c r="AP35" s="11"/>
+      <c r="AQ35" s="12">
         <f>100/Q35</f>
         <v>0.61349693251533743</v>
       </c>
-      <c r="AO35" s="11"/>
-      <c r="AP35" s="11"/>
-      <c r="AQ35" s="11">
-        <f>100/T35</f>
+      <c r="AR35" s="11"/>
+      <c r="AS35" s="11"/>
+      <c r="AT35" s="11"/>
+      <c r="AU35" s="11">
+        <f>100/U35</f>
         <v>1.8796992481203008</v>
       </c>
-      <c r="AR35" s="11"/>
-    </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AV35" s="11"/>
+    </row>
+    <row r="36" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>12</v>
       </c>
@@ -2579,67 +2684,69 @@
       <c r="S36" s="7"/>
       <c r="T36" s="7"/>
       <c r="U36" s="7"/>
-      <c r="Y36" t="str">
+      <c r="V36" s="7"/>
+      <c r="AB36" t="str">
         <f>B36</f>
         <v>NewYork</v>
       </c>
-      <c r="Z36" s="12">
+      <c r="AC36" s="12">
         <f>100/C36</f>
         <v>0.14836795252225518</v>
       </c>
-      <c r="AA36" s="12">
+      <c r="AD36" s="12">
         <f>100/D36</f>
         <v>0.31948881789137379</v>
       </c>
-      <c r="AB36" s="12">
+      <c r="AE36" s="12">
         <f>100/E36</f>
         <v>0.19305019305019305</v>
       </c>
-      <c r="AC36" s="12">
+      <c r="AF36" s="12">
         <f>100/F36</f>
         <v>0.17006802721088435</v>
       </c>
-      <c r="AD36" s="11">
-        <f t="shared" ref="AD36:AD38" si="21">100/G36</f>
+      <c r="AG36" s="11">
+        <f>100/G36</f>
         <v>1.2048192771084338</v>
       </c>
-      <c r="AE36" s="11">
+      <c r="AH36" s="11">
         <f>100/H36</f>
         <v>2.2271714922048997</v>
       </c>
-      <c r="AF36" s="12">
+      <c r="AI36" s="12">
         <f>100/I36</f>
         <v>0.4366812227074236</v>
       </c>
-      <c r="AG36" s="11">
+      <c r="AJ36" s="11">
         <f>100/J36</f>
         <v>1.1534025374855825</v>
       </c>
-      <c r="AH36" s="15">
-        <f t="shared" si="20"/>
+      <c r="AK36" s="15">
+        <f>100/K36</f>
         <v>10.989010989010989</v>
       </c>
-      <c r="AI36" s="11"/>
-      <c r="AJ36" s="11"/>
-      <c r="AK36" s="12">
+      <c r="AL36" s="11"/>
+      <c r="AM36" s="11"/>
+      <c r="AN36" s="12">
         <f>100/N36</f>
         <v>0.4329004329004329</v>
       </c>
-      <c r="AL36" s="12">
+      <c r="AO36" s="12">
         <f>100/O36</f>
         <v>0.44247787610619471</v>
       </c>
-      <c r="AM36" s="12">
-        <f t="shared" ref="AM36" si="22">100/P36</f>
+      <c r="AP36" s="12">
+        <f>100/P36</f>
         <v>0.12376237623762376</v>
       </c>
-      <c r="AN36" s="11"/>
-      <c r="AO36" s="11"/>
-      <c r="AP36" s="11"/>
       <c r="AQ36" s="11"/>
       <c r="AR36" s="11"/>
-    </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AS36" s="11"/>
+      <c r="AT36" s="11"/>
+      <c r="AU36" s="11"/>
+      <c r="AV36" s="11"/>
+    </row>
+    <row r="37" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>8</v>
       </c>
@@ -2664,22 +2771,20 @@
       <c r="S37" s="7"/>
       <c r="T37" s="7"/>
       <c r="U37" s="7"/>
-      <c r="Y37" t="str">
+      <c r="V37" s="7"/>
+      <c r="AB37" t="str">
         <f>B37</f>
         <v>AWS US E1</v>
       </c>
-      <c r="Z37" s="11"/>
-      <c r="AA37" s="11"/>
-      <c r="AB37" s="11"/>
       <c r="AC37" s="11"/>
       <c r="AD37" s="11"/>
-      <c r="AE37" s="11">
+      <c r="AE37" s="11"/>
+      <c r="AF37" s="11"/>
+      <c r="AG37" s="11"/>
+      <c r="AH37" s="11">
         <f>100/H37</f>
         <v>6.2111801242236018</v>
       </c>
-      <c r="AF37" s="11"/>
-      <c r="AG37" s="11"/>
-      <c r="AH37" s="11"/>
       <c r="AI37" s="11"/>
       <c r="AJ37" s="11"/>
       <c r="AK37" s="11"/>
@@ -2690,8 +2795,12 @@
       <c r="AP37" s="11"/>
       <c r="AQ37" s="11"/>
       <c r="AR37" s="11"/>
-    </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AS37" s="11"/>
+      <c r="AT37" s="11"/>
+      <c r="AU37" s="11"/>
+      <c r="AV37" s="11"/>
+    </row>
+    <row r="38" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>6</v>
       </c>
@@ -2743,94 +2852,108 @@
         <v>470</v>
       </c>
       <c r="T38" s="7">
+        <v>345</v>
+      </c>
+      <c r="U38" s="7">
         <v>31.4</v>
       </c>
-      <c r="U38" s="7">
+      <c r="V38" s="7">
         <v>995</v>
       </c>
-      <c r="V38" s="7">
+      <c r="W38" s="7">
         <v>525</v>
       </c>
-      <c r="Y38" t="str">
+      <c r="X38" s="7">
+        <v>475</v>
+      </c>
+      <c r="AB38" t="str">
         <f>B38</f>
         <v>San Diego</v>
       </c>
-      <c r="Z38" s="11"/>
-      <c r="AA38" s="12">
+      <c r="AC38" s="11"/>
+      <c r="AD38" s="12">
         <f>100/D38</f>
         <v>0.20964360587002095</v>
       </c>
-      <c r="AB38" s="12">
+      <c r="AE38" s="12">
         <f>100/E38</f>
         <v>0.2109704641350211</v>
       </c>
-      <c r="AC38" s="12">
+      <c r="AF38" s="12">
         <f>100/F38</f>
         <v>9.5238095238095233E-2</v>
       </c>
-      <c r="AD38" s="11">
-        <f t="shared" si="21"/>
+      <c r="AG38" s="11">
+        <f>100/G38</f>
         <v>4.6296296296296298</v>
       </c>
-      <c r="AE38" s="12">
+      <c r="AH38" s="12">
         <f>100/H38</f>
         <v>0.21598272138228941</v>
       </c>
-      <c r="AF38" s="12">
+      <c r="AI38" s="12">
         <f>100/I38</f>
         <v>0.52083333333333337</v>
       </c>
-      <c r="AG38" s="12">
+      <c r="AJ38" s="12">
         <f>100/J38</f>
         <v>0.47619047619047616</v>
       </c>
-      <c r="AH38" s="11">
-        <f t="shared" ref="AH38" si="23">100/K38</f>
+      <c r="AK38" s="11">
+        <f>100/K38</f>
         <v>7.9365079365079367</v>
       </c>
-      <c r="AI38" s="11"/>
-      <c r="AJ38" s="15">
-        <f t="shared" ref="AJ38" si="24">100/M38</f>
+      <c r="AL38" s="11"/>
+      <c r="AM38" s="15">
+        <f>100/M38</f>
         <v>17.361111111111111</v>
       </c>
-      <c r="AK38" s="11">
-        <f t="shared" ref="AK38" si="25">100/N38</f>
+      <c r="AN38" s="11">
+        <f>100/N38</f>
         <v>7.5757575757575761</v>
       </c>
-      <c r="AL38" s="11">
-        <f t="shared" ref="AL38" si="26">100/O38</f>
+      <c r="AO38" s="11">
+        <f>100/O38</f>
         <v>0.94517958412098302</v>
       </c>
-      <c r="AM38" s="12">
+      <c r="AP38" s="12">
         <f>100/P38</f>
         <v>0.43103448275862066</v>
       </c>
-      <c r="AN38" s="11">
+      <c r="AQ38" s="11">
         <f>100/Q38</f>
         <v>1.1441647597254003</v>
       </c>
-      <c r="AO38" s="12">
+      <c r="AR38" s="12">
         <f>100/R38</f>
         <v>0.10526315789473684</v>
       </c>
-      <c r="AP38" s="12">
-        <f t="shared" ref="AP38:AS40" si="27">100/S38</f>
+      <c r="AS38" s="12">
+        <f>100/S38</f>
         <v>0.21276595744680851</v>
       </c>
-      <c r="AQ38" s="11">
+      <c r="AT38" s="12">
         <f>100/T38</f>
+        <v>0.28985507246376813</v>
+      </c>
+      <c r="AU38" s="11">
+        <f>100/U38</f>
         <v>3.1847133757961785</v>
       </c>
-      <c r="AR38" s="12">
-        <f t="shared" si="27"/>
+      <c r="AV38" s="12">
+        <f>100/V38</f>
         <v>0.10050251256281408</v>
       </c>
-      <c r="AS38" s="12">
-        <f t="shared" si="27"/>
+      <c r="AW38" s="12">
+        <f>100/W38</f>
         <v>0.19047619047619047</v>
       </c>
-    </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AX38" s="12">
+        <f>100/X38</f>
+        <v>0.21052631578947367</v>
+      </c>
+    </row>
+    <row r="39" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>7</v>
       </c>
@@ -2862,52 +2985,54 @@
       </c>
       <c r="S39" s="7"/>
       <c r="T39" s="7"/>
-      <c r="U39" s="7">
+      <c r="U39" s="7"/>
+      <c r="V39" s="7">
         <v>900</v>
       </c>
-      <c r="Y39" t="str">
+      <c r="AB39" t="str">
         <f>B39</f>
         <v>AWS US W2</v>
       </c>
-      <c r="Z39" s="12">
+      <c r="AC39" s="12">
         <f>100/C39</f>
         <v>0.11764705882352941</v>
       </c>
-      <c r="AA39" s="11"/>
-      <c r="AB39" s="11"/>
-      <c r="AC39" s="12">
+      <c r="AD39" s="11"/>
+      <c r="AE39" s="11"/>
+      <c r="AF39" s="12">
         <f>100/F39</f>
         <v>9.2850510677808723E-2</v>
       </c>
-      <c r="AD39" s="11"/>
-      <c r="AE39" s="12">
+      <c r="AG39" s="11"/>
+      <c r="AH39" s="12">
         <f>100/H39</f>
         <v>0.19455252918287938</v>
       </c>
-      <c r="AF39" s="12"/>
-      <c r="AG39" s="12"/>
-      <c r="AH39" s="11"/>
-      <c r="AI39" s="11"/>
-      <c r="AJ39" s="11"/>
+      <c r="AI39" s="12"/>
+      <c r="AJ39" s="12"/>
       <c r="AK39" s="11"/>
       <c r="AL39" s="11"/>
-      <c r="AM39" s="11">
+      <c r="AM39" s="11"/>
+      <c r="AN39" s="11"/>
+      <c r="AO39" s="11"/>
+      <c r="AP39" s="11">
         <f>100/P39</f>
         <v>6.1728395061728394</v>
       </c>
-      <c r="AN39" s="11"/>
-      <c r="AO39" s="12">
+      <c r="AQ39" s="11"/>
+      <c r="AR39" s="12">
         <f>100/R39</f>
         <v>0.12391573729863693</v>
       </c>
-      <c r="AP39" s="12"/>
-      <c r="AQ39" s="12"/>
-      <c r="AR39" s="12">
-        <f t="shared" si="27"/>
+      <c r="AS39" s="12"/>
+      <c r="AT39" s="12"/>
+      <c r="AU39" s="12"/>
+      <c r="AV39" s="12">
+        <f>100/V39</f>
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>17</v>
       </c>
@@ -2924,34 +3049,36 @@
         <v>303</v>
       </c>
       <c r="T40" s="7"/>
-      <c r="Y40" t="str">
+      <c r="U40" s="7"/>
+      <c r="AB40" t="str">
         <f>B40</f>
         <v>Korea</v>
       </c>
-      <c r="AJ40" s="12">
-        <f t="shared" ref="AJ40" si="28">100/M40</f>
+      <c r="AM40" s="12">
+        <f>100/M40</f>
         <v>0.58479532163742687</v>
       </c>
-      <c r="AM40" s="12">
+      <c r="AP40" s="12">
         <f>100/P40</f>
         <v>0.1111111111111111</v>
       </c>
-      <c r="AO40" s="11">
+      <c r="AR40" s="11">
         <f>100/R40</f>
         <v>3.4965034965034962</v>
       </c>
-      <c r="AP40" s="12">
-        <f t="shared" si="27"/>
+      <c r="AS40" s="12">
+        <f>100/S40</f>
         <v>0.33003300330033003</v>
       </c>
-      <c r="AQ40" s="11"/>
-    </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AT40" s="12"/>
+      <c r="AU40" s="11"/>
+    </row>
+    <row r="45" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>21</v>
       </c>

</xml_diff>